<commit_message>
read directly form excel
</commit_message>
<xml_diff>
--- a/stimuli_de/multipleye-stimuli-experiment-de.xlsx
+++ b/stimuli_de/multipleye-stimuli-experiment-de.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tzp466/Documents/research/projects/multipleye/stimulus/final/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0843B030-2CE3-6047-BC60-3FA1203E2531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{0843B030-2CE3-6047-BC60-3FA1203E2531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0AA467DA-DC13-41F1-82B8-B5EE878024A2}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15760" xr2:uid="{EF339F11-F4DE-4D0A-862E-E00578AF5D2A}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="225">
   <si>
     <t>stimulus_id</t>
   </si>
@@ -281,6 +281,345 @@
     <t>correct_answer_key_q5</t>
   </si>
   <si>
+    <t>PopSci_MultiplEYE</t>
+  </si>
+  <si>
+    <t>Willkommen bei MultiplEYE!</t>
+  </si>
+  <si>
+    <t>Der Name „MultiplEYE“ ist ein Wortspiel, das „multilingualism“ (Englisch: Mehrsprachigkeit) oder „multiple languages“ (Englisch: mehrere Sprachen) mit „eye“ (Englisch: Auge) aus „Eye-Tracking“ (Englisch: Blickverfolgung) verbindet. MultiplEYE ist eine von der Europäischen Union finanzierte COST Action. COST Actions sind Forschungsnetzwerke, die von der European Cooperation in Science and Technology, oder kurz COST, unterstützt werden. 
+Als Förderorganisation unterstützt COST unser ständig wachsendes Netzwerk von Forschern in ganz Europa und darüber hinaus, indem es finanzielle Mittel für die Durchführung verschiedener Arten von Networking-Aktivitäten bereitstellt.</t>
+  </si>
+  <si>
+    <t>Zu diesen Aktivitäten gehören Arbeitsgruppentreffen, Weiterbildungskurse, um Expertise an jüngeren Forscher weiterzugeben, und wissenschaftliche Forschungsaufenthalte.
+Der Projekttitel der MultiplEYE COST Action lautet: Ermöglichung der mehrsprachigen Eye-Tracking-Datenerfassung für die menschliche und maschinelle Sprachverarbeitungsforschung (übersetzt aus dem Englischen). Das bedeutet, dass die MultiplEYE COST Action darauf abzielt, ein interdisziplinäres Netzwerk von Forschungsgruppen zu fördern, die an der Erhebung von Augenbewegungsdaten beim Lesen in verschiedenen Sprachen arbeiten.</t>
+  </si>
+  <si>
+    <t>Ziel ist es, die Entwicklung eines großen mehrsprachigen Korpus von Augenbewegungsdaten zu unterstützen und es Forschern zu ermöglichen, Daten zu sammeln, indem sie ihr Expertenwissen aus verschiedenen Disziplinen teilen. Dazu gehören Linguistik, Psychologie, Sprach- und Lesetherapie und Informatik. Diese Datensammlung kann dann verwendet werden, um die menschliche Sprachverarbeitung aus psycholinguistischer Perspektive zu untersuchen, sowie die computergestützte Sprachverarbeitung aus der Perspektive des Maschinellen Lernens zu verbessern und zu evaluieren.</t>
+  </si>
+  <si>
+    <t>Was ist ”Eye-Tracking”?
+Eye-Tracking ist der Prozess, bei dem der Blickpunkt – wohin Sie schauen – und die Augenbewegungen zwischen festen Blickpunkten gemessen werden. Das Gerät, mit dem die Augenpositionen und -bewegungen gemessen werden, wird als Eye-Tracker bezeichnet. Es besteht aus einer Infrarotkamera, die eine Lichtfrequenz verwendet, die das menschliche Auge nicht stört oder verletzt.</t>
+  </si>
+  <si>
+    <t>Mit Hilfe von Bilderkennungsalgorithmen ist der Eye-Tracker in der Lage, Blickpunkte sehr genau zu schätzen, indem er die Position von Kopf und Augen, die Entfernung zum Bildschirm, auf den ein Teilnehmer blickt, und die Position des Eye-Trackers kennt.
+Eye-Tracking ist eine nützliche Technologie für eine Vielzahl von Anwendungen. Beispielsweise kann es dabei helfen, Müdigkeit beim Autofahren zu erkennen oder Anwendungen für Screening- und Trainingszwecke im medizinischen Bereich unterstützen. Eye-Tracking wird auch in der Gaming-Branche, im Marketing und in der Forschung zur Interaktion von Mensch und Maschine eingesetzt.</t>
+  </si>
+  <si>
+    <t>Warum ist Eye-Tracking beim Lesen für unser Projekt besonders interessant?
+Während Sie diese Wörter lesen, folgt der Eye-Tracker Ihren Augenbewegungen über den Text. Dies gibt Aufschluss darüber, wie lange Sie sich einen Text angesehen haben, oder genauer gesagt, wie lange Sie zum Lesen jedes Wortes gebraucht haben, welche Wörter Sie übersprungen haben, bei welchen Wörtern Sie verweilt sind und ob Sie zurückgehen mussten, um die bereits gelesenen Wörter nochmals anzuschauen, um Teile des Textes besser zu verstehen.</t>
+  </si>
+  <si>
+    <t>Während Ihr Gehirn den Inhalt des Textes verarbeitet, spiegeln Ihre Augenbewegungen fast in Echtzeit einen Großteil der dafür benötigten sprachlichen und kognitiven Verarbeitung wider. Die aufgezeichneten Daten sind also eine Goldgrube an Informationen darüber, wie wir die Bedeutung und die grammatikalischen Strukturen eines Textes zusammensetzen. Es zeigt, mit welchen Textstellen wir zu kämpfen haben und welche einfach lesbar sind. Die Forscher können daraus ableiten, welche sprachlichen Faktoren welche Art von Augenbewegungen verursacht haben.</t>
+  </si>
+  <si>
+    <t>Die Motivation hinter MultiplEYE ist, dass Eye-Tracking-Daten noch immer nur spärlich verfügbar sind, insbesondere für kleinere Sprachen. Eine so große Datensammlung ist eine Herausforderung in Bezug auf die Entwicklung und die Vereinbarung des experimentellen Designs, die Komplexität und die Art der Texte, die von den Teilnehmern gelesen werden sollen. Andere Entscheidungen, die weniger relevant erscheinen, aber tatsächlich sehr wichtig sind, betreffen die Schriftart und -größe des Textes, die Reihenfolge der Texte, den Versuchsablauf und die Art und Weise, wie die Daten danach verarbeitet werden.</t>
+  </si>
+  <si>
+    <t>Aber sobald dieser Datensatz fertig ist, wird er es uns ermöglichen, viele Themen im Zusammenhang mit Psycholinguistik und Computerlinguistik zu untersuchen. Beispielsweise können wir das Leseverhalten über verschiedene Sprachen hinweg vergleichen. Hat die Schrift, z.B. das lateinische Alphabet im Vergleich zur kyrillischen oder arabischen Schrift, einen Einfluss auf die Lesezeit? Ein Beispiel für die computergestützte Textverarbeitung könnte die Verwendung von Eye-Tracking-Daten sein, um Anwendungen künstlicher Intelligenz voranzutreiben, die den menschlichen Leseprozess nachahmen. Diese Erkenntnisse könnten verwendet werden, um bessere maschinelle Übersetzungssysteme zu bauen oder um die automatische Extraktion von Schlüsselwörtern aus Texten zu verbessern.</t>
+  </si>
+  <si>
+    <t>Das Erhalten von Eye-Tracking-Daten von vielen verschiedenen Teilnehmern, einschließlich Ihnen selbst, die Texte in vielen verschiedenen Sprachen lesen, wird eine großartige Grundlage für unsere Forschung sein. Sie wird der Hauptfaktor sein, um unser Forschungsnetzwerk zu einem erfolgreichen Unterfangen zu machen.
+Wir hoffen, dass wir den Weg für die Förderung der Forschung in verschiedenen Teilgebieten der Linguistik ebnen können, indem wir eine große Gruppe von Forschern unterstützen und vernetzen.</t>
+  </si>
+  <si>
+    <t>Die Hauptergebnisse der MultiplEYE Action werden ein großer Datensatz mit Blickverfolgungsdaten in vielen Sprachen und eine Plattform für neue Kooperationen sein, die diese Art von Daten nutzen.
+Wenn Sie diesen Text lesen, unterstützen Sie uns bereits, indem Sie uns erlauben, Ihre Augenbewegungen beim Lesen und Verstehen von Sprache zu erfassen und zu analysieren. Vielen Dank!</t>
+  </si>
+  <si>
+    <t>Ins_HumanRights</t>
+  </si>
+  <si>
+    <t>Die Allgemeine Erklärung der Menschenrechte - Präambel</t>
+  </si>
+  <si>
+    <t>Da die Anerkennung der angeborenen Würde und der gleichen und unveräußerlichen Rechte aller Mitglieder der Gemeinschaft der Menschen die Grundlage von Freiheit, Gerechtigkeit und Frieden in der Welt bildet,</t>
+  </si>
+  <si>
+    <t>da die Nichtanerkennung und Verachtung der Menschenrechte zu Akten der Barbarei geführt haben, die das Gewissen der Menschheit mit Empörung erfüllen, und da verkündet worden ist, daß einer Welt, in der die Menschen Rede- und Glaubensfreiheit und Freiheit von Furcht und Not genießen, das höchste Streben des Menschen gilt,</t>
+  </si>
+  <si>
+    <t>da es notwendig ist, die Menschenrechte durch die Herrschaft des Rechtes zu schützen, damit der Mensch nicht gezwungen wird, als letztes Mittel zum Aufstand gegen Tyrannei und Unterdrückung zu greifen,</t>
+  </si>
+  <si>
+    <t>da es notwendig ist, die Entwicklung freundschaftlicher Beziehungen zwischen den Nationen zu fördern,</t>
+  </si>
+  <si>
+    <t>da die Völker der Vereinten Nationen in der Charta ihren Glauben an die grundlegenden Menschenrechte, an die Würde und den Wert der menschlichen Person und an die Gleichberechtigung von Mann und Frau erneut bekräftigt und beschlossen haben, den sozialen Fortschritt und bessere Lebensbedingungen in größerer Freiheit zu fördern,</t>
+  </si>
+  <si>
+    <t>da die Mitgliedstaaten sich verpflichtet haben, in Zusammenarbeit mit den Vereinten Nationen auf die allgemeine Achtung und Einhaltung der Menschenrechte und Grundfreiheiten hinzuwirken,</t>
+  </si>
+  <si>
+    <t>da ein gemeinsames Verständnis dieser Rechte und Freiheiten von größter Wichtigkeit für die volle Erfüllung dieser Verpflichtung ist,</t>
+  </si>
+  <si>
+    <t>verkündet die Generalversammlung diese Allgemeine Erklärung der Menschenrechte als das von allen Völkern und Nationen zu erreichende gemeinsame Ideal, damit jeder einzelne und alle Organe der Gesellschaft sich diese Erklärung stets gegenwärtig halten und sich bemühen, durch Unterricht und Erziehung die Achtung vor diesen Rechten und Freiheiten zu fördern und durch fortschreitende nationale und internationale Maßnahmen ihre allgemeine und tatsächliche Anerkennung und Einhaltung durch die Bevölkerung der Mitgliedstaaten selbst wie auch durch die Bevölkerung der ihrer Hoheitsgewalt unterstehenden Gebiete zu gewährleisten.</t>
+  </si>
+  <si>
+    <t>Ins_EURLex</t>
+  </si>
+  <si>
+    <t>BERICHT DER KOMMISSION AN DEN RAT: Fortschrittsbericht über eine Benchmark für die Lernmobilität</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. EINFÜHRUNG
+In der jüngsten Mitteilung der Kommission „Investieren in Europas Jugend“ werden die positiven Auswirkungen der Lernmobilität auf Beschäftigungsfähigkeit und bürgerschaftliches Engagement hervorgehoben. In einem anderen Land zu lernen, zu studieren oder einer Ausbildung nachzugehen, ist eine einzigartige Erfahrung und kann neue Perspektiven eröffnen. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Die Kompetenzen, die im Rahmen einer Mobilitätserfahrung erworben werden, etwa Problemlösungs- und Anpassungsfähigkeit sowie Toleranz und Zuversicht, werden von Arbeitgebern geschätzt und sind in der heutigen Gesellschaft unentbehrlich.
+Die Kommission fördert die Lernmobilität junger Menschen im Rahmen ihrer politischen Konzepte und Programme, die auch eine spezielle Benchmark und die Unterstützung durch das Programm Erasmus+ umfassen. </t>
+  </si>
+  <si>
+    <t>In seinen Schlussfolgerungen zu einer Benchmark für die Lernmobilität (2011/C 372/08) fordert der Rat die Kommission auf, „dem Rat bis Ende 2015 über die Ergebnisse im Hinblick auf eine Überprüfung und gegebenenfalls Überarbeitung der [...] europäischen Benchmark Bericht zu erstatten“.
+Der Rat fordert die Kommission und die Mitgliedstaaten außerdem zur Durchführung einer Reihe weiterer Maßnahmen auf, die sich insbesondere auf Indikatoren für die Mobilität von Studentinnen und Studenten, jungen Menschen und Lehrkräften beziehen. Im Zusammenhang mit diesen Maßnahmen besteht jedoch keine Verpflichtung zur Berichterstattung an den Rat. Hierzu stehen separate Unterlagen der Kommission zur Verfügung, in denen die Maßnahmen eingehender beschrieben werden.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hintergrund der Schlussfolgerungen des Rates von 2011 ist der strategische Rahmen für die europäische Zusammenarbeit auf dem Gebiet der allgemeinen und beruflichen Bildung 2020, in dem die Kommission ersucht wird, „bis Ende 2010 einen Vorschlag für eine Benchmark in diesem Bereich vorzulegen, der sich zunächst auf die physische Mobilität zwischen Ländern im Bereich der Hochschulbildung konzentrieren [...] sollte.“ Den Schlussfolgerungen des Rates ging eine Arbeitsunterlage der Kommissionsdienststellen vom 24. Mai 2011 zur Entwicklung von Benchmarks zu Bildung für Beschäftigungsfähigkeit und zu Mobilität zu Lernzwecken (Dok. 10697/11) voraus.
+Mit dem vorliegenden Bericht wird die Verpflichtung zur Berichterstattung an den Rat über die erzielten Fortschritte bei der Mobilitätsbenchmark im Hinblick auf die Fortsetzung der Arbeit bis 2020 eingelöst. </t>
+  </si>
+  <si>
+    <t>Die aus zwei Indikatoren bestehende Benchmark für die Lernmobilität wird im Anhang der Schlussfolgerungen von 2011 folgendermaßen definiert:
+– „Bis 2020 sollten in der EU durchschnittlich mindestens 20 % der Hochschulabsolventen eine Studien- oder Ausbildungsphase (einschließlich Praktika) im Ausland absolviert haben, die mindestens 15 ECTS-Leistungspunkte abdeckt oder eine Mindestdauer von 3 Monaten umfasst.“
+– „Bis 2020 sollten in der EU durchschnittlich mindestens 6 % der 18- bis 34-Jährigen mit abgeschlossener beruflicher Erstausbildung eine mit der Berufsausbildung zusammenhängende Ausbildungsphase (einschließlich Praktika) von mindestens zwei Wochen oder, sofern im ‚Europass‘ verzeichnet, auch von kürzerer Dauer im Ausland absolviert haben.“</t>
+  </si>
+  <si>
+    <t>Der Schwerpunkt der Benchmark liegt auf der ausgehenden Mobilität, mit anderen Worten auf dem Ausmaß, in dem Menschen ins Ausland gehen, um Lernerfahrungen und Qualifikationen zu erwerben. Innerhalb der EU steht dieses Ziel mit den Grundsätzen der Freizügigkeit von Personen und Arbeitskräften im Binnenmarkt in Verbindung.</t>
+  </si>
+  <si>
+    <t>Die EU-Benchmark misst die Zahl der Absolventen, die während ihres Studiums mobil waren und ihre Qualifikation erfolgreich abgeschlossen haben. Sie hat keinen direkten Bezug zu einem geografischen Gebiet, in den Schlussfolgerungen von 2011 wird jedoch betont: „Lernmobilität bedeutet physische Mobilität einschließlich weltweiter Mobilität.“ Die Messung des Indikators der Benchmark für die Mobilität in der Berufsausbildung wird in der Praxis durch das in den Schlussfolgerungen genannte Instrument (eine Haushaltserhebung bei einer bestimmten, breit angelegten Altersgruppe) begrenzt, während die Quelle für den Indikator im Bereich der Hochschulbildung nicht festgelegt ist.</t>
+  </si>
+  <si>
+    <t>Lit_Alchemist</t>
+  </si>
+  <si>
+    <t>Der Alchemist - Kapitel 1</t>
+  </si>
+  <si>
+    <t>Der Jüngling hieß Santiago. Es fing bereits an zu dämmern, als er mit seiner Schafherde zu einer alten, verlassenen Kirche kam. Das Dach war schon vor geraumer Zeit eingestürzt, und ein riesiger Maulbeerbaum wuchs an jener Stelle, wo sich einst die Sakristei befand.
+Er entschloß sich, die Nacht hier zu verbringen. So geleitete er alle Schafe durch die beschädigte Türe und legte einige Bretter quer davor, damit ihm die Tiere während der Nacht nicht entwischen konnten.</t>
+  </si>
+  <si>
+    <t>Zwar gab es keine Wölfe in jener Gegend, aber einmal war ihm eines der Tiere während der Nacht entkommen, und er mußte den ganzen folgenden Tag mit der Suche nach dem verirrten Schäfchen verbringen.
+Danach breitete er seinen Mantel auf dem Fußboden aus, legte sich nieder und nahm das Buch, das er gerade gelesen hatte, als Kopfkissen. Vor dem Einschlafen dachte er daran, daß er in Zukunft dickere Bücher lesen wollte, weil man länger etwas davon hat und weil sie eine bequemere Kopfstütze abgeben.</t>
+  </si>
+  <si>
+    <t>Es war noch finster, als er erwachte. Als er nach oben schaute, sah er die Sterne zwischen den Dachbalken durchscheinen.
+"Eigentlich wollte ich noch weiterschlafen", dachte er bei sich. Wieder hatte er den gleichen Traum gehabt wie vor einer Woche, und wieder war er vor dem Ende aufgewacht.
+Er erhob sich und trank einen Schluck Wein. Dann nahm er seinen Hirtenstab und begann, die Schafe, die noch schliefen, eines nach dem anderen zu wecken. Mehr und mehr wurden die Tiere, wie ihm aufgefallen war, gleichzeitig mit ihm wach, als ob ein geheimnisvoller Gleichklang sein Leben mit dem der Schafe verband, die seit nunmehr zwei Jahren mit ihm übers Land gezogen waren, auf der Suche nach Wasser und Nahrung.</t>
+  </si>
+  <si>
+    <t>"Sie haben sich schon so an mich gewöhnt, daß sie meinen Rhythmus kennen", dachte er. Aber nach kurzer Überlegung kam er zu dem Schluß, daß es auch umgekehrt sein könnte: Er selber hatte sich dem Rhythmus seiner Schafe angepaßt!
+Einige unter den Tieren brauchten etwas länger zum Aufstehen. Der Jüngling weckte sie mit seinem Stab, indem er jedes bei seinem Namen nannte. Immer hatte er den Eindruck, daß die Schafe alles verstanden, was er sagte. Darum las er ihnen auch gelegentlich Abschnitte aus Büchern vor, die ihn besonders beeindruckten, oder er philosophierte über die Einsamkeit und die Freuden eines Schafhirten, oder er kommentierte die letzten Neuigkeiten, die er im den Städten erfahren hatte, durch die er zu ziehen pflegte.</t>
+  </si>
+  <si>
+    <t>Seit zwei Tagen jedoch sprach er beinahe nur noch über eins: die Tochter eines Händlers, die in jener Kleinstadt lebte, welche sie in vier Tagen erreichen würden. Im vorigen Jahr war er das erste Mal bei diesem Handelsmann gewesen, der Besitzer eines Textilgeschäftes war und darauf bestand, daß die Schafe vor seinem Geschäft geschoren würden, um jeden Betrug zu vermeiden. Ein Bekannt er hatte den Laden empfohlen, und so brachte der Hirte seine Schafe jetzt dorthin.</t>
+  </si>
+  <si>
+    <t>Lit_Emperor_Clothes</t>
+  </si>
+  <si>
+    <t>Des Kaisers Neue Kleider</t>
+  </si>
+  <si>
+    <t>Vor vielen Jahren lebte ein Kaiser, der so ungeheuer viel auf neue Kleider hielt, daß er all sein Geld dafür ausgab, um recht geputzt zu sein. Er kümmerte sich nicht um seine Soldaten, kümmerte sich nicht um Theater und liebte es nicht, in den Wald zu fahren, außer um seine neuen Kleider zu zeigen. Er hatte einen Rock für jede Stunde des Tages, und ebenso wie man von einem König sagte, er ist im Rat, so sagte man hier immer: "Der Kaiser ist in der Garderobe!"</t>
+  </si>
+  <si>
+    <t>In der großen Stadt, in der er wohnte, ging es sehr munter her. An jedem Tag kamen viele Fremde an, und eines Tages kamen auch zwei Betrüger, die gaben sich für Weber aus und sagten, daß sie das schönste Zeug, was man sich denken könne, zu weben verstanden. Die Farben und das Muster seien nicht allein ungewöhnlich schön, sondern die Kleider, die von dem Zeuge genäht würden, sollten die wunderbare Eigenschaft besitzen, daß sie für jeden Menschen unsichtbar seien, der nicht für sein Amt tauge oder der unverzeihlich dumm sei.</t>
+  </si>
+  <si>
+    <t>,Das wären ja prächtige Kleider', dachte der Kaiser; wenn ich solche hätte, könnte ich ja dahinterkommen, welche Männer in meinem Reiche zu dem Amte, das sie haben, nicht taugen, ich könnte die Klugen von den Dummen unterscheiden! Ja, das Zeug muß sogleich für mich gewebt werden!' Er gab den beiden Betrügern viel Handgeld, damit sie ihre Arbeit beginnen sollten.</t>
+  </si>
+  <si>
+    <t>Sie stellten auch zwei Webstühle auf, taten, als ob sie arbeiteten, aber sie hatten nicht das geringste auf dem Stuhle. Trotzdem verlangten sie die feinste Seide und das prächtigste Gold, das steckten sie aber in ihre eigene Tasche und arbeiteten an den leeren Stühlen bis spät in die Nacht hinein.
+,Nun möchte ich doch wissen, wie weit sie mit dem Zeuge sind!' dachte der Kaiser, aber es war ihm beklommen zumute, wenn er daran dachte, daß keiner, der dumm sei oder schlecht zu seinem Amte tauge, es sehen könne. Er glaubte zwar, daß er für sich selbst nichts zu fürchten brauche, aber er wollte doch erst einen andern senden, um zu sehen, wie es damit stehe.</t>
+  </si>
+  <si>
+    <t>Alle Menschen in der ganzen Stadt wußten, welche besondere Kraft das Zeug habe, und alle waren begierig zu sehen, wie schlecht oder dumm ihr Nachbar sei.
+,Ich will meinen alten, ehrlichen Minister zu den Webern senden', dachte der Kaiser, er kann am besten beurteilen, wie der Stoff sich ausnimmt, denn er hat Verstand, und keiner versieht sein Amt besser als er!'
+Nun ging der alte, gute Minister in den Saal hinein, wo die zwei Betrüger saßen und an den leeren Webstühlen arbeiteten. ,Gott behüte uns!' dachte der alte Minister und riß die Augen auf. ,Ich kann ja nichts erblicken!' Aber das sagte er nicht.</t>
+  </si>
+  <si>
+    <t>Beide Betrüger baten ihn näher zu treten und fragten, ob es nicht ein hübsches Muster und schöne Farben seien. Dann zeigten sie auf den leeren Stuhl, und der arme, alte Minister fuhr fort, die Augen aufzureißen, aber er konnte nichts sehen, denn es war nichts da. ,Herr Gott', dachte er, sollte ich dumm sein? Das habe ich nie geglaubt, und das darf kein Mensch wissen! Sollte ich nicht zu meinem Amte taugen? Nein, es geht nicht an, daß ich erzähle, ich könne das Zeug nicht sehen!'
+"Nun, Sie sagen nichts dazu?" fragte der eine von den Webern.</t>
+  </si>
+  <si>
+    <t>"Oh, es ist niedlich, ganz allerliebst!" antwortete der alte Minister und sah durch seine Brille. "Dieses Muster und diese Farben! – Ja, ich werde dem Kaiser sagen, daß es mir sehr gefällt!"
+"Nun, das freut uns!" sagten beide Weber, und darauf benannten sie die Farben mit Namen und erklärten das seltsame Muster. Der alte Minister merkte gut auf, damit er dasselbe sagen könne, wenn er zum Kaiser zurückkomme, und das tat er auch.
+Nun verlangten die Betrüger mehr Geld, mehr Seide und mehr Gold zum Weben. Sie steckten alles in ihre eigenen Taschen, auf den Webstuhl kam kein Faden, aber sie fuhren fort, wie bisher an den leeren Stühlen zu arbeiten.</t>
+  </si>
+  <si>
+    <t>Sie steckten alles in ihre eigenen Taschen, auf den Webstuhl kam kein Faden, aber sie fuhren fort, wie bisher an den leeren Stühlen zu arbeiten.
+Der Kaiser sandte bald wieder einen anderen tüchtigen Staatsmann hin, um zu sehen, wie es mit dem Weben stehe und ob das Zeug bald fertig sei; es ging ihm aber gerade wie dem ersten, er guckte und guckte; weil aber außer dem Webstuhl nichts da war, so konnte er nichts sehen.
+"Ist das nicht ein ganz besonders prächtiges und hübsches Stück Zeug?" fragten die beiden Betrüger und zeigten und erklärten das prächtige Muster, das gar nicht da war.</t>
+  </si>
+  <si>
+    <t>,Dumm bin ich nicht', dachte der Mann; es ist also mein gutes Amt, zu dem ich nicht tauge! Das wäre seltsam genug, aber das muß man sich nicht merken lassen!' Daher lobte er das Zeug, das er nicht sah, und versicherte ihnen seine Freude über die schönen Farben und das herrliche Muster. "Ja, es ist ganz allerliebst!" sagte er zum Kaiser.
+Alle Menschen in der Stadt sprachen von dem prächtigen Zeuge.</t>
+  </si>
+  <si>
+    <t>Nun wollte der Kaiser es selbst sehen, während es noch auf dem Webstuhl sei. Mit einer ganzen Schar auserwählter Männer, unter denen auch die beiden ehrlichen Staatsmänner waren, die schon früher dagewesen, ging er zu den beiden listigen Betrügern hin, die nun aus allen Kräften webten, aber ohne Faser oder Faden.
+"Ja, ist das nicht prächtig?" sagten die beiden ehrlichen Staatsmänner. "Wollen Eure Majestät sehen, welches Muster, welche Farben?" und dann zeigten sie auf den leeren Webstuhl, denn sie glaubten, daß die andern das Zeug wohl sehen könnten.</t>
+  </si>
+  <si>
+    <t>,Was!' dachte der Kaiser; ich sehe gar nichts! Das ist ja erschrecklich! Bin ich dumm? Tauge ich nicht dazu, Kaiser zu sein? Das wäre das Schrecklichste, was mir begegnen könnte.' "Oh, es ist sehr hübsch", sagte er; "es hat meinen allerhöchsten Beifall!" und er nickte zufrieden und betrachtete den leeren Webstuhl; er wollte nicht sagen, daß er nichts sehen könne. Das ganze Gefolge, was er mit sich hatte, sah und sah, aber es bekam nicht mehr heraus als alle die andern, aber sie sagten gleich wie der Kaiser: "Oh, das ist hübsch!' und sie rieten ihm, diese neuen prächtigen Kleider das erste Mal bei dem großen Feste, das bevorstand, zu tragen.</t>
+  </si>
+  <si>
+    <t>"Es ist herrlich, niedlich, ausgezeichnet!" ging es von Mund zu Mund, und man schien allerseits innig erfreut darüber. Der Kaiser verlieh jedem der Betrüger ein Ritterkreuz, um es in das Knopfloch zu hängen, und den Titel Hofweber.
+Die ganze Nacht vor dem Morgen, an dem das Fest stattfinden sollte, waren die Betrüger auf und hatten sechzehn Lichte angezündet, damit man sie auch recht gut bei ihrer Arbeit beobachten konnte. Die Leute konnten sehen, daß sie stark beschäftigt waren, des Kaisers neue Kleider fertigzumachen. Sie taten, als ob sie das Zeug aus dem Webstuhl nähmen, sie schnitten in die Luft mit großen Scheren, sie nähten mit Nähnadeln ohne Faden und sagten zuletzt: "Sieh, nun sind die Kleider fertig!"</t>
+  </si>
+  <si>
+    <t>Der Kaiser mit seinen vornehmsten Beamten kam selbst, und beide Betrüger hoben den einen Arm in die Höhe, gerade, als ob sie etwas hielten, und sagten: "Seht, hier sind die Beinkleider, hier ist das Kleid, hier ist der Mantel!" und so weiter. "Es ist so leicht wie Spinnwebe; man sollte glauben, man habe nichts auf dem Körper, aber das ist gerade die Schönheit dabei!"
+"Ja!" sagten alle Beamten, aber sie konnten nichts sehen, denn es war nichts da.</t>
+  </si>
+  <si>
+    <t>"Belieben Eure Kaiserliche Majestät Ihre Kleider abzulegen", sagten die Betrüger, "so wollen wir Ihnen die neuen hier vor dem großen Spiegel anziehen!"
+Der Kaiser legte seine Kleider ab, und die Betrüger stellten sich, als ob sie ihm ein jedes Stück der neuen Kleider anzogen, die fertig genäht sein sollten, und der Kaiser wendete und drehte sich vor dem Spiegel.
+"Ei, wie gut sie kleiden, wie herrlich sie sitzen!" sagten alle. "Welches Muster, welche Farben! Das ist ein kostbarer Anzug!" –</t>
+  </si>
+  <si>
+    <t>"Draußen stehen sie mit dem Thronhimmel, der über Eurer Majestät getragen werden soll!" meldete der Oberzeremonienmeister.
+"Seht, ich bin ja fertig!" sagte der Kaiser. "Sitzt es nicht gut?" und dann wendete er sich nochmals zu dem Spiegel; denn es sollte scheinen, als ob er seine Kleider recht betrachte.</t>
+  </si>
+  <si>
+    <t>Die Kammerherren, die das Recht hatten, die Schleppe zu tragen, griffen mit den Händen gegen den Fußboden, als ob sie die Schleppe aufhöben, sie gingen und taten, als hielten sie etwas in der Luft; sie wagten es nicht, es sich merken zu lassen, daß sie nichts sehen konnten.
+So ging der Kaiser unter dem prächtigen Thronhimmel, und alle Menschen auf der Straße und in den Fenstern sprachen: "Wie sind des Kaisers neue Kleider unvergleichlich! Welche Schleppe er am Kleide hat! Wie schön sie sitzt!" Keiner wollte es sich merken lassen, daß er nichts sah; denn dann hätte er ja nicht zu seinem Amte getaugt oder wäre sehr dumm gewesen.</t>
+  </si>
+  <si>
+    <t>Keine Kleider des Kaisers hatten solches Glück gemacht wie diese.
+"Aber er hat ja gar nichts an!" sagte endlich ein kleines Kind. "Hört die Stimme der Unschuld!" sagte der Vater; und der eine zischelte dem andern zu, was das Kind gesagt hatte.
+"Aber er hat ja gar nichts an!" rief zuletzt das ganze Volk. Das ergriff den Kaiser, denn das Volk schien ihm recht zu haben, aber er dachte bei sich: ,Nun muß ich aushalten.' Und die Kammerherren gingen und trugen die Schleppe, die gar nicht da war.</t>
+  </si>
+  <si>
+    <t>Lit_Harry_Potter</t>
+  </si>
+  <si>
+    <t>Harry Potter und der Stein der Weisen - Kapitel 1: Ein Junge überlebt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mr und Mrs Dursley im Ligusterweg Nummer 4 waren stolz darauf, ganz und gar normal zu sein, sehr stolz sogar. Niemand wäre auf die Idee gekommen, sie könnten sich in eine merkwürdige und geheimnisvolle Geschichte verstricken, denn mit solchem Unsinn wollten sie nichts zu tun haben. </t>
+  </si>
+  <si>
+    <t>Mr Dursley war Direktor einer Firma namens Grunnings, die Bohrmaschinen herstellte. Er war groß und bullig und hatte fast keinen Hals, dafür aber einen sehr großen Schnurrbart. Mrs Dursley war dünn und blond und besaß doppelt so viel Hals, wie notwendig gewesen wäre, was allerdings sehr nützlich war, denn so konnte sie den Hals über den Gartenzaun recken und zu den Nachbarn hinüberspähen. Die Dursleys hatten einen kleinen Sohn namens Dudley und in ihren Augen gab es nirgendwo einen prächtigeren Jungen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Die Dursleys besaßen alles, was sie wollten, doch sie hatten auch ein Geheimnis, und dass es jemand aufdecken könnte, war ihre größte Sorge. Einfach unerträglich wäre es, wenn die Sache mit den Potters herauskommen würde. Mrs Potter war die Schwester von Mrs Dursley; doch die beiden hatten sich schon seit etlichen Jahren nicht mehr gesehen. Mrs Dursley behauptete sogar, dass sie gar keine Schwester hätte, denn diese und deren Nichtsnutz von einem Mann waren so undursleyhaft, wie man es sich nur denken konnte. </t>
+  </si>
+  <si>
+    <t>Die Dursleys schauderten beim Gedanken daran, was die Nachbarn sagen würden, sollten die Potters eines Tages in ihrer Straße aufkreuzen. Die Dursleys wussten, dass auch die Potters einen kleinen Sohn hatten, doch den hatten sie nie gesehen. Auch dieser Junge war ein guter Grund, sich von den Potters fernzuhalten; mit einem solchen Kind sollte ihr Dudley nicht in Berührung kommen.</t>
+  </si>
+  <si>
+    <t>Als Mr und Mrs Dursley an dem trüben und grauen Dienstag, an dem unsere Geschichte beginnt, die Augen aufschlugen, war an dem wolkenverhangenen Himmel draußen kein Vorzeichen der merkwürdigen und geheimnisvollen Dinge zu erkennen, die bald überall im Land geschehen sollten. Mr Dursley summte vor sich hin und suchte sich für die Arbeit seine langweiligste Krawatte aus, und Mrs Dursley schwatzte munter vor sich hin, während sie mit dem schreienden Dudley rangelte und ihn in seinen Hochstuhl zwängte.</t>
+  </si>
+  <si>
+    <t>Keiner von ihnen sah den riesigen Waldkauz am Fenster vorbeifliegen.
+Um halb neun griff Mr Dursley nach der Aktentasche, gab seiner Frau einen Schmatz auf die Wange und versuchte es auch bei Dudley mit einem Abschiedskuss. Der ging jedoch daneben, weil Dudley gerade einen Wutanfall hatte und die Wände mit seinem Haferbrei bewarf. »Kleiner Schlingel«, gluckste Mr Dursley, während er nach draußen ging. Er setzte sich in den Wagen und fuhr rückwärts die Einfahrt zu Nummer 4 hinaus.</t>
+  </si>
+  <si>
+    <t>Lit_MagicMountain</t>
+  </si>
+  <si>
+    <t>Der Zauberberg - Vorsatz</t>
+  </si>
+  <si>
+    <t>Die Geschichte Hans Castorps, die wir erzählen wollen, – nicht um seinetwillen (denn der Leser wird einen einfachen, wenn auch ansprechenden jungen Menschen in ihm kennenlernen), sondern um der Geschichte willen, die uns in hohem Grade erzählenswert scheint (wobei zu Hans Castorps Gunsten denn doch erinnert werden sollte, daß es seine Geschichte ist, und daß nicht jedem jede Geschichte passiert): diese Geschichte ist sehr lange her, sie ist sozusagen schon ganz mit historischem Edelrost überzogen und unbedingt in der Zeitform der tiefsten Vergangenheit vorzutragen.</t>
+  </si>
+  <si>
+    <t>Das wäre kein Nachteil für eine Geschichte, sondern eher ein Vorteil; denn Geschichten müssen vergangen sein, und je vergangener, könnte man sagen, desto besser für sie in ihrer Eigenschaft als Geschichten und für den Erzähler, den raunenden Beschwörer des Imperfekts. Es steht jedoch so mit ihr, wie es heute auch mit den Menschen und unter diesen nicht zum wenigsten mit den Geschichtenerzählern steht: sie ist viel älter als ihre Jahre, ihre Betagtheit ist nicht nach Tagen, das Alter, das auf ihr liegt, nicht nach Sonnenumläufen zu berechnen; mit einem Worte: sie verdankt den Grad ihres Vergangenseins nicht eigentlich der Zeit, – eine Aussage, womit auf die Fragwürdigkeit und eigentümliche Zwienatur dieses geheimnisvollen Elementes im Vorbeigehen angespielt und hingewiesen sei.</t>
+  </si>
+  <si>
+    <t>Um aber einen klaren Sachverhalt nicht künstlich zu verdunkeln: die hochgradige Verflossenheit unserer Geschichte rührt daher, daß sie vor einer gewissen, Leben und Bewußtsein tief zerklüftenden Wende und Grenze spielt ... Sie spielt, oder, um jedes Präsens geflissentlich zu vermeiden, sie spielte und hat gespielt vormals, ehedem, in den alten Tagen, der Welt vor dem großen Kriege, mit dessen Beginn so vieles begann, was zu beginnen wohl kaum schon aufgehört hat. Vorher also spielt sie, wenn auch nicht lange vorher. Aber ist der Vergangenheitscharakter einer Geschichte nicht desto tiefer, vollkommener und märchenhafter, je dichter „vorher“ sie spielt? Zudem könnte es sein, daß die unsrige mit dem Märchen auch sonst, ihrer inneren Natur nach, das eine und andre zu schaffen hat.</t>
+  </si>
+  <si>
+    <t>Wir werden sie ausführlich erzählen, genau und gründlich, – denn wann wäre je die Kurz- oder Langweiligkeit einer Geschichte abhängig gewesen von dem Raum und der Zeit, die sie in Anspruch nahm? Ohne Furcht vor dem Odium der Peinlichkeit, neigen wir vielmehr der Ansicht zu, daß nur das Gründliche wahrhaft unterhaltend sei.</t>
+  </si>
+  <si>
+    <t>Im Handumdrehen also wird der Erzähler mit Hansens Geschichte nicht fertig werden. Die sieben Tage einer Woche werden dazu nicht reichen und auch sieben Monate nicht. Am besten ist es, er macht sich im voraus nicht klar, wieviel Erdenzeit ihm verstreichen wird, während sie ihn umsponnen hält. Es werden, in Gottes Namen, ja nicht geradezu sieben Jahre sein!</t>
+  </si>
+  <si>
+    <t>Lit_NorthWind</t>
+  </si>
+  <si>
+    <t>Der Nordwind und die Sonne</t>
+  </si>
+  <si>
+    <t>Einst stritten sich Nordwind und Sonne, wer von ihnen beiden wohl der Stärkere wäre, als ein Wanderer, der in einen warmen Mantel gehüllt war, des Weges daherkam. Sie wurden einig, dass derjenige für den Stärkeren gelten sollte, der den Wanderer zwingen würde, seinen Mantel abzunehmen. Der Nordwind blies mit aller Macht, aber je mehr er blies, desto fester hüllte sich der anderer in seinen Mantel ein. Endlich gab der Nordwind den Kampf auf. Nun erwärmte die Sonne die Luft mit ihren freundlichen Strahlen, und schon nach wenigen Augenblicken zog der Wanderer seinen Mantel aus. Da musste der Nordwind zugeben, dass die Sonne von ihnen beiden der Stärkere war.</t>
+  </si>
+  <si>
+    <t>Lit_Solaris</t>
+  </si>
+  <si>
+    <t>Solaris - Kapitel 2: Die Solaristen</t>
+  </si>
+  <si>
+    <t>Die Entdeckung der Solaris erfolgte nahezu hundert Jahre, bevor ich geboren wurde.
+Der Planet kreist um zwei Sonnen, eine rote und eine blaue. Über vierzig Jahre lang näherte sich ihm kein Raumschiff, die Gamov-Shapleysche Theorie über die Unmöglichkeit der Entstehung von Leben auf Planeten von Doppelsternen galt damals für erwiesen. Die Bahnen solcher Planeten ändern sich unentwegt infolge des Wechselspiels der Massenanziehungen, das vor sich geht, während die beiden Sonnen einander umkreisen.</t>
+  </si>
+  <si>
+    <t>Die entstehenden Perturbationen kürzen und längen abwechselnd die Bahn des Planeten, und sollten Urkeim e von Leben entstehen, so unterliegen sie der Zerstörung durch glutheiße Strahlung oder auch durch eisige Kälte. Diese Änderungen vollziehen sich im Zeitraum von Jahrmillionen, also der astronomischen oder biologischen Größenordnung nach (da die Evolution hunderte Millionen, wenn nicht eine Milliarde von Jahren erfordert) - in sehr kurzer Zeit.</t>
+  </si>
+  <si>
+    <t>Nach den ursprünglichen Berechnungen sollte sich die Solaris im Lauf von fünfhunderttausend Jahren bis auf die Distanz  von einer halben astronomischen Einheit ihrer roten Sonne nähern und nach einer weiter en Million - in ihren Glutenabgrund stürzen. 
+Aber schon nach etwas mehr als zehn Jahren überzeugte man sich, daß die Solarisbahn keineswegs die erwarteten Änderungen aufwies, ganz als ob sie konstant wäre, so konstant wie die Bahnen der Planeten unseres Sonnensystems.</t>
+  </si>
+  <si>
+    <t>Man wiederholte, nun schon mit höchster Genauigkeit, die Beobachtungen und Messungen, die nur bestätigten, was bekannt war: die Solaris besitzt eine unbeständige Umlaufbahn.
+Von einem unter etlichen hundert neuentdeckten Planeten pro Jahr, die mit Notizen von ein paar Zeilen, mit Angabe der Elemente ihrer Bewegung, in die großen Statistiken einbezogen werden, avancierte die Solaris nun in den Rang eines besonderer Beachtung würdigen Himmelskörpers.</t>
+  </si>
+  <si>
+    <t>Und so kreiste denn an die vier Jahre nach dieser Entdeckung Ottenskjolds Expedition um den Planeten und untersuchte ihn vom Laokoon und von zwei Begleitschiffen aus. Diese Expedition hatte den Charakter provisorischer, improvisierter Auskundschaftung, zumal da sie nicht zum Landen ausgerüstet war. Sie brachte in Äquator- und Pol-Umlaufbahnen eine größere Anzahl von Beobachtungssatelliten an, deren Hauptaufgabe die Messung der Gravitationspotentiale war.</t>
+  </si>
+  <si>
+    <t>Überdies wurden die fast gänzlich vom Ozean bedeckte Planetenoberfläche und die wenigen aus seinem Niveau herausragenden Hochebenen erforscht. Diese erreichen insgesamt nicht den Flächeninhalt Europas, obwohl die Solaris um zwanzig Prozent größeren Durchmesser hat als die Erde. Diese unregelmäßig verstreuten Brocken von felsigem und ödem Land häufen sich vor allem auf der Südhalbkugel.</t>
+  </si>
+  <si>
+    <t>Man stellte auch die Zusammensetzung der Atmosphäre fest, die keinen Sauerstoff enthält, und maß überaus genau die Dichte des Planeten sowie die Albedo und andere astronomische Elemente. Wie erwartet, wurden keine Spuren von Leben aufgefunden, weder an Land, noch gewahrte man welche am Ozean.</t>
+  </si>
+  <si>
+    <t>Während weiterer zehn Jahre zeigte die Solaris, nun schon im Zentrum der Aufmerksamkeit aller Observatorien dieses Bereichs, erstaunliche Tendenz zur Beibehaltung ihrer außer allem Zweifel gravitationsmäßig unbeständigen Umlaufbahn. Eine Zeit lang roch die Angelegenheit nach Skandal, denn die Schuld an einem solchen Beobachtungsergebnis suchte man (immer aus Sorge um das Wohl der Wissenschaft) bald auf bestimmte Leute zu schieben, bald auf die Rechenanlagen, deren sie sich bedienten.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Der Mangel an Geldmitteln zögerte die Entsendung einer eigentlichen Solaris-Expedition weitere drei Jahre hinaus, bis zu dem Zeitpunkt, da Shannahan die Besatzung komplett hatte und vom Institut drei Einheiten der Tonnage C, Kosmodromklasse, erlangte. Anderthalb Jahre vor Eintreffen der Expedition, die vom Gebiet des Alpha des Wassermanns aus startete, brachte von seiten des Instituts eine zweite Explorationsflotte ein automatisches Satelloid, Luna 247, in eine Solaris-Umlaufbahn. </t>
+  </si>
+  <si>
+    <t>Nach dreijahrzehntelang auseinanderliegenden Rekonstruktionen arbeitet dieses Satelloid heute noch. Die Daten, die es sammelte, bestätigten endgültig, was Ottenskjolds Expedition wahrgenommen hatte: den aktiven Charakter der Ozeanbewegungen.
+Ein Schiff Shannahans verblieb auf einer hohen Umlaufbahn, zwei dagegen landeten nach einleitenden Vorbereitungen auf einem felsigen Stück Land, das beim Südpol der Solaris etwa sechshundert Quadratmeilen einnimmt.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Die Arbeiten der Expedition waren nach achtzehn Monaten beendet und verliefen günstig, bis auf einen Unglücksfall, der durch Fehlfunktion der Apparate verursacht wurde. Innerhalb des Wissenschaftlerteams kam es jedoch zur Aufspaltung in zwei gegnerische Lager. Zum Gegenstand des Streits wurde der Ozean. Auf Grund der Analysen wurde er als organisches Gebilde erkannt (ihn lebendig zu nennen, wagte damals noch niemand). </t>
+  </si>
+  <si>
+    <t>Während jedoch die Biologen in ihm ein primitives Gebilde sahen - eine Art gigantischen Verband, also gleichsam eine einzige monströs auseinandergewachsene flüssige Zelle (aber sie nannten ihn `präbiologische Formation´), die den ganzen Globus mit einem gallertigen, stellenweise eine Tiefe von mehreren Meilen erreichenden Mantel überzogen hat - behaupteten Astronomen und Physiker, das müsse eine außerordentlich hoch organisierte Struktur sein, die möglicher weise an Verschlungenheit des Aufbaus die irdischen Organismen übertreffe, da sie doch imstande sei, aktiv die Ausformung der Planetenbahn zu beeinflussen.</t>
+  </si>
+  <si>
+    <t>Es wurde nämlich keinerlei andere Ursache entdeckt, die das Verhalten der Solaris erklärt hätte; überdies fanden die Planetarphysiker eine Beziehung zwischen bestimmten Prozessendes Plasma-Ozeans und dem örtlich gemessenen Gravitationspotential, das sich in Abhängigkeit vom Ozean-eigenen ` Stoffwechsel´ änderte.
+So brachten also Physiker und nicht Biologen die paradoxe Formulierung `plasmatische Maschine´ vor; darunter verstanden sie ein Gebilde, in unserem Sinne vielleicht auch unbelebt, doch fähig, zielbezogene Tätigkeiten zu unternehmen - fügen wir gleich hinzu: in astronomischer Größenordnung.</t>
+  </si>
+  <si>
+    <t>In diesem Streit, der innerhalb von Wochen die bedeutendsten Autoritäten sämtlich in seinen Wirbel hineinzog, geriet zum ersten Mal seit achtzig Jahren die Gamov-Shapleysche Doktrin ins Wanken.
+Eine Zeitlang suchte man sie noch zu verteidigen, indem man behauptete, der Ozeanhabe nichts mit Leben zu tun, er sei nicht einmal ein `para´- oder `prä´-biologisches Gebilde, sondern eine geologische Formation, gewiß ungewöhnlich, aber nur zur Fixierung der Solarisbahn durch Schwerkraftänderungen fähig, wobei man sich auf die Le-Chateliersche Regel berief.</t>
+  </si>
+  <si>
+    <t>Solchem Konservatismus zum Trotz erwuchsen Hypothesen, wie etwa eine der besser ausgearbeiteten, von Civito und Vitta, der Ozean sei das Ergebnis dialektischer Entwicklung: aus seiner Vorform, dem Ur-Ozean, einer Lösung träge reagierender chemischer Körper, vermochte er unter dem Druck der Verhältnisse (das heißt, der Bahnänderungen, die seine Existenz bedrohten) ohne alle Zwischenstufen irdischer Entwicklung, also ohne das Entstehen von Ein- und Vielzellern, ohne pflanzliche und tierische Evolution, ohne das Auftreten von Nervensystem und Gehirn, gleich in das Stadium des `homöostatischen Ozeans´ umzuspringen.</t>
+  </si>
+  <si>
+    <t>Das heißt mit anderen Worten, daß er sich nicht wie die irdischen Organismen hunderte Jahrmillionen lang an die Umwelt anpaßte, um erst nach einer so enormen Zeitspanne eine intelligente Rasse zu erzeugen, sondern sofort seine Umwelt bewältigte.
+Das war durchaus originell, bloß wußte weiterhin niemand, wie eine sirupartige Gallerte die Bahn eines Himmelskörpers stabilisieren kann. Seit fast hundert Jahren kannte man Anlagen zur Herstellung künstlicher Kraft- und Schwerefelder, die Gravitoren, aber niemand konnte sich auch nur vorstellen, wie ein Resultat, das - in den Gravitoren ñ das Ergebnis komplizierter Kernreaktionen und enormer Temperaturen ist, von einem gestaltlosen Brei zustande gebracht werden kann.</t>
+  </si>
+  <si>
+    <t>In den Zeitungen, die damals zur Kurzweil der Leser und zum Grauen der Wissenschaftler nur so strotzten von hanebüchenen Schwindeleien zum Thema `Geheimnis der Solaris´, fehlte es auch nicht an Behauptungen, der planetare Ozean sei ... ein entfernter Verwandter der irdischen elektrischen Zitteraale.
+Als es gelang, das Problem zumindest einigermaßen zu entwirren, erwies sich, daß die Erklärung, wie dies bei der Solaris später noch oft vorkam, an die Stelle eines Rätsels ein anderes, vielleicht noch erstaunlicheres, setzte.</t>
+  </si>
+  <si>
+    <t>Die Untersuchungen ergaben, daß der Ozean keineswegs nach dem Prinzip unserer Gravitoren funktioniert (was im übrigen unmöglich wäre), sondern direkt die Raum-Zeit-Metrik zu modellieren vermag, was unter anderem zu Abweichungen in der Zeitmessung an einem und demselben Längengrad der Solaris führt. Demnach kannte der Ozean nicht nur in gewissem Sinne die Einstein-Boevische Theorie, sondern vermochte sogar (was man von uns nicht sagen kann), ihre Konsequenzen zu nutzen.</t>
+  </si>
+  <si>
+    <t>Als dies ausgesprochen war, brach in der wissenschaftlichen Welt einer der heftigsten Stürme unseres Jahrhunderts los. Die ehrwürdigsten, allgemein als Wahrheiten anerkannten Theorien stürzten zu Schutt zusammen, in der wissenschaftlichen Literatur tauchten die ketzerischsten Artikel auf, und die Alternative `genialer Ozean´ oder `Graviations-Gallerte´ erhitzte alle Gemüter.</t>
+  </si>
+  <si>
+    <t>Lit_BrokenApril</t>
+  </si>
+  <si>
     <t>multiple choice</t>
   </si>
   <si>
@@ -338,40 +677,64 @@
     <t>answer_option_3_1</t>
   </si>
   <si>
-    <t>Lit_Alchemist</t>
-  </si>
-  <si>
-    <t>Lit_Emperor_Clothes</t>
-  </si>
-  <si>
-    <t>Lit_Harry_Potter</t>
-  </si>
-  <si>
-    <t>Lit_Solaris</t>
-  </si>
-  <si>
     <t>Arg_PisaRapaNui</t>
   </si>
   <si>
+    <t>Die Osterinsel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Einleitung
+Stell dir vor, dass eine örtliche Bibliothek nächste Woche zu einem Vortrag einlädt. Der Vortrag wird von einer Professorin einer nahegelegenen Universität gehalten. Sie wird über ihre Feldforschung auf der Osterinsel sprechen, die im pazifischen Ozean, über 3200 Kilometer westlich von Chile, liegt.
+</t>
+  </si>
+  <si>
+    <t>Deine Klasse wird den Vortrag besuchen. Euer Geschichtslehrer bittet euch die Geschichte der Osterinsel zu recherchieren, damit ihr etwas darüber wisst, bevor ihr den Vortrag besucht.
+Die erste Quelle, die du lesen wirst, ist ein Blogeintrag, der von der Professorin geschrieben wurde, während sie auf der Osterinsel lebte.</t>
+  </si>
+  <si>
+    <t>www.dieprofessorinblog.de/feldforschung/osterinsel
+Blog der Professorin
+Gepostet am 23. Mai, 11:22 Uhr</t>
+  </si>
+  <si>
+    <t>Während ich heute Morgen aus meinem Fenster schaue, sehe ich die Landschaft, die ich zu lieben gelernt habe, hier auf Rapa Nui, mancherorts auch Osterinsel genannt. Die Gräser und Büsche sind grün, der Himmel ist blau und die alten, jetzt erloschenen Vulkane erheben sich im Hintergrund.</t>
+  </si>
+  <si>
+    <t>Ich bin ein bisschen traurig, weil ich weiß, dass dies meine letzte Woche auf der Insel ist. Ich habe meine Feldforschung abgeschlossen und werde nach Hause zurückkehren. Nachher werde ich noch einen Spaziergang durch die Hügel machen und mich von den Moai verabschieden, die ich in den letzten neun Monaten erforscht habe. Hier ist ein Bild von einigen dieser riesigen Statuen.</t>
+  </si>
+  <si>
+    <t>Wenn Sie meinen Blog dieses Jahr verfolgt haben, dann wissen Sie, dass die Menschen der Osterinsel diese Moai vor Hunderten von Jahren gemeißelt haben. Diese beeindruckenden Moai wurden in einem einzigen Steinbruch im östlichen Teil der Insel gemeißelt. Einige von ihnen wogen Tausende von Kilos, trotzdem waren die Menschen der Osterinsel in der Lage, sie ohne Kräne oder jegliche schwere Ausrüstung an Orte zu transportieren, die weit entfernt vom Steinbruch waren.</t>
+  </si>
+  <si>
+    <t>Jahrelang wussten Archäologen nicht, wie diese riesigen Statuen transportiert wurden. Es blieb bis in die 1990er Jahre ein Rätsel, als schließlich ein Team von Archäologen und Bewohnern der Osterinsel zeigte, dass die Moai mithilfe von Seilen aus Pflanzen und hölzernen Rollen und Schienen aus großen Bäumen, die früher zahlreich auf der Insel gewachsen waren, transportiert und aufgestellt worden sein könnten. Das Rätsel der Moai war gelöst.</t>
+  </si>
+  <si>
+    <t>Ein anderes Rätsel blieb jedoch. Was geschah mit diesen Pflanzen und großen Bäumen, die verwendet worden waren, um die Moai zu transportieren? Wie bereits erwähnt, sehe ich, wenn ich aus meinem Fenster schaue, Gräser und Büsche und ein oder zwei kleine Bäume, aber nichts, was hätte verwendet werden können, um diese riesigen Statuen zu transportieren. Es ist ein faszinierendes Geheimnis, eines das ich in zukünftigen Posts und Vorträgen erforschen werde. Bis dahin wollen Sie vielleicht dem Rätsel selbst auf den Grund gehen. Ich schlage vor, Sie beginnen mit dem Buch „Kollaps” von Jared Diamond. Diese Buchbesprechung von „Kollaps” ist ein guter Anfang.</t>
+  </si>
+  <si>
+    <t>Reisender_14 24. Mai, 16:31 Uhr
+"Hallo Frau Professor! Ich verfolge Ihre Arbeit auf der Osterinsel mit Begeisterung. Ich kann es kaum erwarten, einen Blick in „Kollaps” zu werfen!"
+KB_Insel 25. Mai, 9:07 Uhr
+"Ich lese auch mit Begeisterung über Ihre Erfahrungen auf der Osterinsel, aber ich glaube, es gibt noch eine andere Theorie, die berücksichtigt werden sollte. Schauen Sie sich diesen Artikel an: www.neuesausderwissenschaft.com/Polynesische_Ratten_Osterinsel"</t>
+  </si>
+  <si>
+    <t>www.wissenschaftliche-buchbesprechung.de/Kollaps
+Buchbesprechung von „Kollaps”</t>
+  </si>
+  <si>
+    <t>Jared Diamonds neues Buch „Kollaps” ist eine eindeutige Warnung vor den Folgen der Zerstörung unserer Umwelt. In dem Buch beschreibt der Autor den Kollaps mehrerer Zivilisationen aufgrund der Entscheidungen, die sie trafen, und deren Auswirkung auf die Umwelt. Eines der beunruhigendsten Beispiele in dem Buch ist die Osterinsel.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Laut dem Autor wurde die Osterinsel irgendwann nach 700 n. Chr. von den Polynesiern besiedelt. Sie entwickelten sich zu einer florierenden Gesellschaft von vielleicht 15.000 Menschen. Sie meißelten die Moai, die berühmten Statuen, und nutzten die verfügbaren natürlichen Ressourcen, um diese riesigen Moai an verschiedene Orte auf der Insel zu transportieren. Als die ersten Europäer 1722 auf die Osterinsel kamen, waren die Moai immer noch dort, aber die Bäume waren verschwunden. </t>
+  </si>
+  <si>
+    <t>Die Bevölkerung war auf wenige Tausend Menschen geschrumpft, die ums Überleben kämpften. Jared Diamond schreibt, dass die Menschen der Osterinsel das Land für landwirtschaftliche und andere Zwecke rodeten und übermäßige Jagd auf die zahlreichen Arten von See- und Landvögeln machten, die auf der Insel lebten. Er vermutet, dass die schwindenden natürlichen Ressourcen zu Stammeskriegen und dem Untergang der Gesellschaft auf der Osterinsel führten.</t>
+  </si>
+  <si>
+    <t>Die Lektion dieses wundervollen, aber beängstigenden Buches ist, dass die Menschen in der Vergangenheit die Entscheidung trafen, ihre Umwelt zu zerstören, indem sie alle Bäume fällten und Tierarten bis zur Ausrottung jagten. Optimistisch weist der Autor darauf hin, dass wir uns entscheiden können, dieselben Fehler heute nicht zu machen. Das Buch ist gut geschrieben und ist es wert, von allen gelesen zu werden, denen die Umwelt am Herzen liegt.</t>
+  </si>
+  <si>
     <t>Arg_PisaCowsMilk</t>
-  </si>
-  <si>
-    <t>PopSci_MultiplEYE</t>
-  </si>
-  <si>
-    <t>Ins_HumanRights</t>
-  </si>
-  <si>
-    <t>Ins_EURLex</t>
-  </si>
-  <si>
-    <t>Lit_MagicMountain</t>
-  </si>
-  <si>
-    <t>Lit_NorthWind</t>
-  </si>
-  <si>
-    <t>Lit_BrokenApril</t>
   </si>
   <si>
     <t>Kuhmilch</t>
@@ -424,373 +787,13 @@
   </si>
   <si>
     <t>Dies sind schwerwiegende Behauptungen und weitere Studien werden benötigt, um die Befunde zu bestätigen. Allerdings häufen sich die Hinweise darauf, dass das Trinken von Kuhmilch möglicherweise weniger gesund ist als urprünglich gedacht. Sollten diese Behauptungen zu unbestrittenen Tatsachen werden, dann könnte es Zeit sein, einfach ‚Nein’ zu Kuhmilch zu sagen.</t>
-  </si>
-  <si>
-    <t>Die Osterinsel</t>
-  </si>
-  <si>
-    <t>Einleitung
-Stell dir vor, dass eine örtliche Bibliothek nächste Woche zu einem Vortrag einlädt. Der Vortrag wird von einer Professorin einer nahegelegenen Universität gehalten. Sie wird über ihre Feldforschung auf der Osterinsel sprechen, die im pazifischen Ozean, über 3200 Kilometer westlich von Chile, liegt.
-Deine Klasse wird den Vortrag besuchen. Euer Geschichtslehrer bittet euch die Geschichte der Osterinsel zu recherchieren, damit ihr etwas darüber wisst, bevor ihr den Vortrag besucht.
-Die erste Quelle, die du lesen wirst, ist ein Blogeintrag, der von der Professorin geschrieben wurde, während sie auf der Osterinsel lebte.</t>
-  </si>
-  <si>
-    <t>www.dieprofessorinblog.de/feldforschung/osterinsel
-Blog der Professorin
-Gepostet am 23. Mai, 11:22 Uhr</t>
-  </si>
-  <si>
-    <t>Während ich heute Morgen aus meinem Fenster schaue, sehe ich die Landschaft, die ich zu lieben gelernt habe, hier auf Rapa Nui, mancherorts auch Osterinsel genannt. Die Gräser und Büsche sind grün, der Himmel ist blau und die alten, jetzt erloschenen Vulkane erheben sich im Hintergrund.</t>
-  </si>
-  <si>
-    <t>Ich bin ein bisschen traurig, weil ich weiß, dass dies meine letzte Woche auf der Insel ist. Ich habe meine Feldforschung abgeschlossen und werde nach Hause zurückkehren. Nachher werde ich noch einen Spaziergang durch die Hügel machen und mich von den Moai verabschieden, die ich in den letzten neun Monaten erforscht habe. Hier ist ein Bild von einigen dieser riesigen Statuen.</t>
-  </si>
-  <si>
-    <t>Wenn Sie meinen Blog dieses Jahr verfolgt haben, dann wissen Sie, dass die Menschen der Osterinsel diese Moai vor Hunderten von Jahren gemeißelt haben. Diese beeindruckenden Moai wurden in einem einzigen Steinbruch im östlichen Teil der Insel gemeißelt. Einige von ihnen wogen Tausende von Kilos, trotzdem waren die Menschen der Osterinsel in der Lage, sie ohne Kräne oder jegliche schwere Ausrüstung an Orte zu transportieren, die weit entfernt vom Steinbruch waren.</t>
-  </si>
-  <si>
-    <t>Jahrelang wussten Archäologen nicht, wie diese riesigen Statuen transportiert wurden. Es blieb bis in die 1990er Jahre ein Rätsel, als schließlich ein Team von Archäologen und Bewohnern der Osterinsel zeigte, dass die Moai mithilfe von Seilen aus Pflanzen und hölzernen Rollen und Schienen aus großen Bäumen, die früher zahlreich auf der Insel gewachsen waren, transportiert und aufgestellt worden sein könnten. Das Rätsel der Moai war gelöst.</t>
-  </si>
-  <si>
-    <t>Ein anderes Rätsel blieb jedoch. Was geschah mit diesen Pflanzen und großen Bäumen, die verwendet worden waren, um die Moai zu transportieren? Wie bereits erwähnt, sehe ich, wenn ich aus meinem Fenster schaue, Gräser und Büsche und ein oder zwei kleine Bäume, aber nichts, was hätte verwendet werden können, um diese riesigen Statuen zu transportieren. Es ist ein faszinierendes Geheimnis, eines das ich in zukünftigen Posts und Vorträgen erforschen werde. Bis dahin wollen Sie vielleicht dem Rätsel selbst auf den Grund gehen. Ich schlage vor, Sie beginnen mit dem Buch „Kollaps” von Jared Diamond. Diese Buchbesprechung von „Kollaps” ist ein guter Anfang.</t>
-  </si>
-  <si>
-    <t>Reisender_14 24. Mai, 16:31 Uhr
-"Hallo Frau Professor! Ich verfolge Ihre Arbeit auf der Osterinsel mit Begeisterung. Ich kann es kaum erwarten, einen Blick in „Kollaps” zu werfen!"
-KB_Insel 25. Mai, 9:07 Uhr
-"Ich lese auch mit Begeisterung über Ihre Erfahrungen auf der Osterinsel, aber ich glaube, es gibt noch eine andere Theorie, die berücksichtigt werden sollte. Schauen Sie sich diesen Artikel an: www.neuesausderwissenschaft.com/Polynesische_Ratten_Osterinsel"</t>
-  </si>
-  <si>
-    <t>www.wissenschaftliche-buchbesprechung.de/Kollaps
-Buchbesprechung von „Kollaps”</t>
-  </si>
-  <si>
-    <t>Jared Diamonds neues Buch „Kollaps” ist eine eindeutige Warnung vor den Folgen der Zerstörung unserer Umwelt. In dem Buch beschreibt der Autor den Kollaps mehrerer Zivilisationen aufgrund der Entscheidungen, die sie trafen, und deren Auswirkung auf die Umwelt. Eines der beunruhigendsten Beispiele in dem Buch ist die Osterinsel.</t>
-  </si>
-  <si>
-    <t>Laut dem Autor wurde die Osterinsel irgendwann nach 700 n. Chr. von den Polynesiern besiedelt. Sie entwickelten sich zu einer florierenden Gesellschaft von vielleicht 15.000 Menschen. Sie meißelten die Moai, die berühmten Statuen, und nutzten die verfügbaren natürlichen Ressourcen, um diese riesigen Moai an verschiedene Orte auf der Insel zu transportieren. Als die ersten Europäer 1722 auf die Osterinsel kamen, waren die Moai immer noch dort, aber die Bäume waren verschwunden. Die Bevölkerung war auf wenige Tausend Menschen geschrumpft, die ums Überleben kämpften. Jared Diamond schreibt, dass die Menschen der Osterinsel das Land für landwirtschaftliche und andere Zwecke rodeten und übermäßige Jagd auf die zahlreichen Arten von See- und Landvögeln machten, die auf der Insel lebten. Er vermutet, dass die schwindenden natürlichen Ressourcen zu Stammeskriegen und dem Untergang der Gesellschaft auf der Osterinsel führten.</t>
-  </si>
-  <si>
-    <t>Die Lektion dieses wundervollen, aber beängstigenden Buches ist, dass die Menschen in der Vergangenheit die Entscheidung trafen, ihre Umwelt zu zerstören, indem sie alle Bäume fällten und Tierarten bis zur Ausrottung jagten. Optimistisch weist der Autor darauf hin, dass wir uns entscheiden können, dieselben Fehler heute nicht zu machen. Das Buch ist gut geschrieben und ist es wert, von allen gelesen zu werden, denen die Umwelt am Herzen liegt.</t>
-  </si>
-  <si>
-    <t>Solaris - Kapitel 2: Die Solaristen</t>
-  </si>
-  <si>
-    <t>Die Entdeckung der Solaris erfolgte nahezu hundert Jahre, bevor ich geboren wurde.
-Der Planet kreist um zwei Sonnen, eine rote und eine blaue. Über vierzig Jahre lang näherte sich ihm kein Raumschiff, die Gamov-Shapleysche Theorie über die Unmöglichkeit der Entstehung von Leben auf Planeten von Doppelsternen galt damals für erwiesen. Die Bahnen solcher Planeten ändern sich unentwegt infolge des Wechselspiels der Massenanziehungen, das vor sich geht, während die beiden Sonnen einander umkreisen.</t>
-  </si>
-  <si>
-    <t>Die entstehenden Perturbationen kürzen und längen abwechselnd die Bahn des Planeten, und sollten Urkeim e von Leben entstehen, so unterliegen sie der Zerstörung durch glutheiße Strahlung oder auch durch eisige Kälte. Diese Änderungen vollziehen sich im Zeitraum von Jahrmillionen, also der astronomischen oder biologischen Größenordnung nach (da die Evolution hunderte Millionen, wenn nicht eine Milliarde von Jahren erfordert) - in sehr kurzer Zeit.</t>
-  </si>
-  <si>
-    <t>Nach den ursprünglichen Berechnungen sollte sich die Solaris im Lauf von fünfhunderttausend Jahren bis auf die Distanz  von einer halben astronomischen Einheit ihrer roten Sonne nähern und nach einer weiter en Million - in ihren Glutenabgrund stürzen. 
-Aber schon nach etwas mehr als zehn Jahren überzeugte man sich, daß die Solarisbahn keineswegs die erwarteten Änderungen aufwies, ganz als ob sie konstant wäre, so konstant wie die Bahnen der Planeten unseres Sonnensystems.</t>
-  </si>
-  <si>
-    <t>Man wiederholte, nun schon mit höchster Genauigkeit, die Beobachtungen und Messungen, die nur bestätigten, was bekannt war: die Solaris besitzt eine unbeständige Umlaufbahn.
-Von einem unter etlichen hundert neuentdeckten Planeten pro Jahr, die mit Notizen von ein paar Zeilen, mit Angabe der Elemente ihrer Bewegung, in die großen Statistiken einbezogen werden, avancierte die Solaris nun in den Rang eines besonderer Beachtung würdigen Himmelskörpers.</t>
-  </si>
-  <si>
-    <t>Und so kreiste denn an die vier Jahre nach dieser Entdeckung Ottenskjolds Expedition um den Planeten und untersuchte ihn vom Laokoon und von zwei Begleitschiffen aus. Diese Expedition hatte den Charakter provisorischer, improvisierter Auskundschaftung, zumal da sie nicht zum Landen ausgerüstet war. Sie brachte in Äquator- und Pol-Umlaufbahnen eine größere Anzahl von Beobachtungssatelliten an, deren Hauptaufgabe die Messung der Gravitationspotentiale war.</t>
-  </si>
-  <si>
-    <t>Überdies wurden die fast gänzlich vom Ozean bedeckte Planetenoberfläche und die wenigen aus seinem Niveau herausragenden Hochebenen erforscht. Diese erreichen insgesamt nicht den Flächeninhalt Europas, obwohl die Solaris um zwanzig Prozent größeren Durchmesser hat als die Erde. Diese unregelmäßig verstreuten Brocken von felsigem und ödem Land häufen sich vor allem auf der Südhalbkugel.</t>
-  </si>
-  <si>
-    <t>Man stellte auch die Zusammensetzung der Atmosphäre fest, die keinen Sauerstoff enthält, und maß überaus genau die Dichte des Planeten sowie die Albedo und andere astronomische Elemente. Wie erwartet, wurden keine Spuren von Leben aufgefunden, weder an Land, noch gewahrte man welche am Ozean.</t>
-  </si>
-  <si>
-    <t>Während weiterer zehn Jahre zeigte die Solaris, nun schon im Zentrum der Aufmerksamkeit aller Observatorien dieses Bereichs, erstaunliche Tendenz zur Beibehaltung ihrer außer allem Zweifel gravitationsmäßig unbeständigen Umlaufbahn. Eine Zeit lang roch die Angelegenheit nach Skandal, denn die Schuld an einem solchen Beobachtungsergebnis suchte man (immer aus Sorge um das Wohl der Wissenschaft) bald auf bestimmte Leute zu schieben, bald auf die Rechenanlagen, deren sie sich bedienten.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Der Mangel an Geldmitteln zögerte die Entsendung einer eigentlichen Solaris-Expedition weitere drei Jahre hinaus, bis zu dem Zeitpunkt, da Shannahan die Besatzung komplett hatte und vom Institut drei Einheiten der Tonnage C, Kosmodromklasse, erlangte. Anderthalb Jahre vor Eintreffen der Expedition, die vom Gebiet des Alpha des Wassermanns aus startete, brachte von seiten des Instituts eine zweite Explorationsflotte ein automatisches Satelloid, Luna 247, in eine Solaris-Umlaufbahn. </t>
-  </si>
-  <si>
-    <t>Nach dreijahrzehntelang auseinanderliegenden Rekonstruktionen arbeitet dieses Satelloid heute noch. Die Daten, die es sammelte, bestätigten endgültig, was Ottenskjolds Expedition wahrgenommen hatte: den aktiven Charakter der Ozeanbewegungen.
-Ein Schiff Shannahans verblieb auf einer hohen Umlaufbahn, zwei dagegen landeten nach einleitenden Vorbereitungen auf einem felsigen Stück Land, das beim Südpol der Solaris etwa sechshundert Quadratmeilen einnimmt.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Die Arbeiten der Expedition waren nach achtzehn Monaten beendet und verliefen günstig, bis auf einen Unglücksfall, der durch Fehlfunktion der Apparate verursacht wurde. Innerhalb des Wissenschaftlerteams kam es jedoch zur Aufspaltung in zwei gegnerische Lager. Zum Gegenstand des Streits wurde der Ozean. Auf Grund der Analysen wurde er als organisches Gebilde erkannt (ihn lebendig zu nennen, wagte damals noch niemand). </t>
-  </si>
-  <si>
-    <t>Während jedoch die Biologen in ihm ein primitives Gebilde sahen - eine Art gigantischen Verband, also gleichsam eine einzige monströs auseinandergewachsene flüssige Zelle (aber sie nannten ihn `präbiologische Formation´), die den ganzen Globus mit einem gallertigen, stellenweise eine Tiefe von mehreren Meilen erreichenden Mantel überzogen hat - behaupteten Astronomen und Physiker, das müsse eine außerordentlich hoch organisierte Struktur sein, die möglicher weise an Verschlungenheit des Aufbaus die irdischen Organismen übertreffe, da sie doch imstande sei, aktiv die Ausformung der Planetenbahn zu beeinflussen.</t>
-  </si>
-  <si>
-    <t>Es wurde nämlich keinerlei andere Ursache entdeckt, die das Verhalten der Solaris erklärt hätte; überdies fanden die Planetarphysiker eine Beziehung zwischen bestimmten Prozessendes Plasma-Ozeans und dem örtlich gemessenen Gravitationspotential, das sich in Abhängigkeit vom Ozean-eigenen ` Stoffwechsel´ änderte.
-So brachten also Physiker und nicht Biologen die paradoxe Formulierung `plasmatische Maschine´ vor; darunter verstanden sie ein Gebilde, in unserem Sinne vielleicht auch unbelebt, doch fähig, zielbezogene Tätigkeiten zu unternehmen - fügen wir gleich hinzu: in astronomischer Größenordnung.</t>
-  </si>
-  <si>
-    <t>In diesem Streit, der innerhalb von Wochen die bedeutendsten Autoritäten sämtlich in seinen Wirbel hineinzog, geriet zum ersten Mal seit achtzig Jahren die Gamov-Shapleysche Doktrin ins Wanken.
-Eine Zeitlang suchte man sie noch zu verteidigen, indem man behauptete, der Ozeanhabe nichts mit Leben zu tun, er sei nicht einmal ein `para´- oder `prä´-biologisches Gebilde, sondern eine geologische Formation, gewiß ungewöhnlich, aber nur zur Fixierung der Solarisbahn durch Schwerkraftänderungen fähig, wobei man sich auf die Le-Chateliersche Regel berief.</t>
-  </si>
-  <si>
-    <t>Solchem Konservatismus zum Trotz erwuchsen Hypothesen, wie etwa eine der besser ausgearbeiteten, von Civito und Vitta, der Ozean sei das Ergebnis dialektischer Entwicklung: aus seiner Vorform, dem Ur-Ozean, einer Lösung träge reagierender chemischer Körper, vermochte er unter dem Druck der Verhältnisse (das heißt, der Bahnänderungen, die seine Existenz bedrohten) ohne alle Zwischenstufen irdischer Entwicklung, also ohne das Entstehen von Ein- und Vielzellern, ohne pflanzliche und tierische Evolution, ohne das Auftreten von Nervensystem und Gehirn, gleich in das Stadium des `homöostatischen Ozeans´ umzuspringen.</t>
-  </si>
-  <si>
-    <t>Das heißt mit anderen Worten, daß er sich nicht wie die irdischen Organismen hunderte Jahrmillionen lang an die Umwelt anpaßte, um erst nach einer so enormen Zeitspanne eine intelligente Rasse zu erzeugen, sondern sofort seine Umwelt bewältigte.
-Das war durchaus originell, bloß wußte weiterhin niemand, wie eine sirupartige Gallerte die Bahn eines Himmelskörpers stabilisieren kann. Seit fast hundert Jahren kannte man Anlagen zur Herstellung künstlicher Kraft- und Schwerefelder, die Gravitoren, aber niemand konnte sich auch nur vorstellen, wie ein Resultat, das - in den Gravitoren ñ das Ergebnis komplizierter Kernreaktionen und enormer Temperaturen ist, von einem gestaltlosen Brei zustande gebracht werden kann.</t>
-  </si>
-  <si>
-    <t>In den Zeitungen, die damals zur Kurzweil der Leser und zum Grauen der Wissenschaftler nur so strotzten von hanebüchenen Schwindeleien zum Thema `Geheimnis der Solaris´, fehlte es auch nicht an Behauptungen, der planetare Ozean sei ... ein entfernter Verwandter der irdischen elektrischen Zitteraale.
-Als es gelang, das Problem zumindest einigermaßen zu entwirren, erwies sich, daß die Erklärung, wie dies bei der Solaris später noch oft vorkam, an die Stelle eines Rätsels ein anderes, vielleicht noch erstaunlicheres, setzte.</t>
-  </si>
-  <si>
-    <t>Die Untersuchungen ergaben, daß der Ozean keineswegs nach dem Prinzip unserer Gravitoren funktioniert (was im übrigen unmöglich wäre), sondern direkt die Raum-Zeit-Metrik zu modellieren vermag, was unter anderem zu Abweichungen in der Zeitmessung an einem und demselben Längengrad der Solaris führt. Demnach kannte der Ozean nicht nur in gewissem Sinne die Einstein-Boevische Theorie, sondern vermochte sogar (was man von uns nicht sagen kann), ihre Konsequenzen zu nutzen.</t>
-  </si>
-  <si>
-    <t>Als dies ausgesprochen war, brach in der wissenschaftlichen Welt einer der heftigsten Stürme unseres Jahrhunderts los. Die ehrwürdigsten, allgemein als Wahrheiten anerkannten Theorien stürzten zu Schutt zusammen, in der wissenschaftlichen Literatur tauchten die ketzerischsten Artikel auf, und die Alternative `genialer Ozean´ oder `Graviations-Gallerte´ erhitzte alle Gemüter.</t>
-  </si>
-  <si>
-    <t>Einst stritten sich Nordwind und Sonne, wer von ihnen beiden wohl der Stärkere wäre, als ein Wanderer, der in einen warmen Mantel gehüllt war, des Weges daherkam.
-Sie wurden einig, dass derjenige für den Stärkeren gelten sollte, der den Wanderer zwingen würde, seinen Mantel abzunehmen.
-Der Nordwind blies mit aller Macht, aber je mehr er blies, desto fester hüllte sich der anderer in seinen Mantel ein.
-Endlich gab der Nordwind den Kampf auf. Nun erwärmte die Sonne die Luft mit ihren
-freundlichen Strahlen, und schon nach wenigen Augenblicken zog der Wanderer seinen Mantel aus.
-Da musste der Nordwind zugeben, dass die Sonne von ihnen beiden der Stärkere war.</t>
-  </si>
-  <si>
-    <t>Der Nordwind und die Sonne</t>
-  </si>
-  <si>
-    <t>Der Zauberberg - Vorsatz</t>
-  </si>
-  <si>
-    <t>Die Geschichte Hans Castorps, die wir erzählen wollen, – nicht um seinetwillen (denn der Leser wird einen einfachen, wenn auch ansprechenden jungen Menschen in ihm kennenlernen), sondern um der Geschichte willen, die uns in hohem Grade erzählenswert scheint (wobei zu Hans Castorps Gunsten denn doch erinnert werden sollte, daß es seine Geschichte ist, und daß nicht jedem jede Geschichte passiert): diese Geschichte ist sehr lange her, sie ist sozusagen schon ganz mit historischem Edelrost überzogen und unbedingt in der Zeitform der tiefsten Vergangenheit vorzutragen.</t>
-  </si>
-  <si>
-    <t>Das wäre kein Nachteil für eine Geschichte, sondern eher ein Vorteil; denn Geschichten müssen vergangen sein, und je vergangener, könnte man sagen, desto besser für sie in ihrer Eigenschaft als Geschichten und für den Erzähler, den raunenden Beschwörer des Imperfekts. Es steht jedoch
-so mit ihr, wie es heute auch mit den Menschen und unter diesen nicht zum wenigsten mit den Geschichtenerzählern steht: sie ist viel älter als ihre Jahre, ihre Betagtheit ist nicht nach Tagen, das Alter, das auf ihr liegt, nicht nach Sonnenumläufen zu berechnen; mit einem Worte: sie
-verdankt den Grad ihres Vergangenseins nicht eigentlich der Zeit, – eine Aussage, womit auf die Fragwürdigkeit und eigentümliche Zwienatur dieses geheimnisvollen Elementes im Vorbeigehen angespielt und hingewiesen sei.</t>
-  </si>
-  <si>
-    <t>Um aber einen klaren Sachverhalt nicht künstlich zu verdunkeln: die hochgradige Verflossenheit unserer Geschichte rührt daher, daß sie vor einer gewissen, Leben und Bewußtsein tief zerklüftenden Wende und Grenze spielt ... Sie spielt, oder, um jedes Präsens geflissentlich zu vermeiden, sie spielte und hat gespielt vormals, ehedem, in den alten Tagen, der Welt vor dem großen Kriege, mit dessen Beginn so vieles begann, was zu beginnen wohl kaum schon aufgehört hat. Vorher also spielt sie, wenn auch nicht lange vorher. Aber ist der Vergangenheitscharakter einer Geschichte nicht desto tiefer, vollkommener und märchenhafter, je dichter „vorher“ sie spielt? Zudem könnte es sein, daß die unsrige mit dem Märchen auch sonst, ihrer inneren Natur nach, das eine und andre zu schaffen hat.</t>
-  </si>
-  <si>
-    <t>Wir werden sie ausführlich erzählen, genau und gründlich, – denn wann wäre je die Kurz- oder Langweiligkeit einer Geschichte abhängig gewesen von dem Raum und der Zeit, die sie in Anspruch nahm? Ohne Furcht vor dem Odium der Peinlichkeit, neigen wir vielmehr der Ansicht zu, daß nur das Gründliche wahrhaft unterhaltend sei.</t>
-  </si>
-  <si>
-    <t>Im Handumdrehen also wird der Erzähler mit Hansens Geschichte nicht fertig werden. Die sieben Tage einer Woche werden dazu nicht reichen und auch sieben Monate nicht. Am besten ist es, er macht sich im voraus nicht klar, wieviel Erdenzeit ihm verstreichen wird, während sie ihn umsponnen hält. Es werden, in Gottes Namen, ja nicht geradezu sieben Jahre sein!</t>
-  </si>
-  <si>
-    <t>Harry Potter und der Stein der Weisen - Kapitel 1: Ein Junge überlebt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mr und Mrs Dursley im Ligusterweg Nummer 4 waren stolz darauf, ganz und gar normal zu sein, sehr stolz sogar. Niemand wäre auf die Idee gekommen, sie könnten sich in eine merkwürdige und geheimnisvolle Geschichte verstricken, denn mit solchem Unsinn wollten sie nichts zu tun haben. </t>
-  </si>
-  <si>
-    <t>Mr Dursley war Direktor einer Firma namens Grunnings, die Bohrmaschinen herstellte. Er war groß und bullig und hatte fast keinen Hals, dafür aber einen sehr großen Schnurrbart. Mrs Dursley war dünn und blond und besaß doppelt so viel Hals, wie notwendig gewesen wäre, was allerdings sehr nützlich war, denn so konnte sie den Hals über den Gartenzaun recken und zu den Nachbarn hinüberspähen. Die Dursleys hatten einen kleinen Sohn namens Dudley und in ihren Augen gab es nirgendwo einen prächtigeren Jungen.</t>
-  </si>
-  <si>
-    <t>Die Dursleys besaßen alles, was sie wollten, doch sie hatten auch ein Geheimnis, und dass es jemand aufdecken könnte, war ihre größte Sorge. Einfach unerträglich wäre es, wenn die Sache mit den Potters herauskommen würde. Mrs Potter war die Schwester von Mrs Dursley; doch die beiden hatten sich schon seit etlichen Jahren nicht mehr gesehen. Mrs Dursley behauptete sogar, dass sie gar keine Schwester hätte, denn diese und deren Nichtsnutz von einem Mann waren so undursleyhaft, wie man es sich nur denken konnte. Die Dursleys schauderten beim Gedanken daran, was die Nachbarn sagen würden, sollten die Potters eines Tages in ihrer Straße aufkreuzen. Die Dursleys wussten, dass auch die Potters einen kleinen Sohn hatten, doch den hatten sie nie gesehen. Auch dieser Junge war ein guter Grund, sich von den Potters fernzuhalten; mit einem solchen Kind sollte ihr Dudley nicht in Berührung kommen.</t>
-  </si>
-  <si>
-    <t>Als Mr und Mrs Dursley an dem trüben und grauen Dienstag, an dem unsere Geschichte beginnt, die Augen aufschlugen, war an dem wolkenverhangenen Himmel draußen kein Vorzeichen der merkwürdigen und geheimnisvollen Dinge zu erkennen, die bald überall im Land geschehen sollten. Mr Dursley summte vor sich hin und suchte sich für die Arbeit seine langweiligste Krawatte aus, und Mrs Dursley schwatzte munter vor sich hin, während sie mit dem schreienden Dudley rangelte und ihn in seinen Hochstuhl zwängte.</t>
-  </si>
-  <si>
-    <t>Keiner von ihnen sah den riesigen Waldkauz am Fenster vorbeifliegen.
-Um halb neun griff Mr Dursley nach der Aktentasche, gab seiner Frau einen Schmatz auf die Wange und versuchte es auch bei Dudley mit einem Abschiedskuss. Der ging jedoch daneben, weil Dudley gerade einen Wutanfall hatte und die Wände mit seinem Haferbrei bewarf. »Kleiner Schlingel«, gluckste Mr Dursley, während er nach draußen ging. Er setzte sich in den Wagen und fuhr rückwärts die Einfahrt zu Nummer 4 hinaus.</t>
-  </si>
-  <si>
-    <t>Des Kaisers Neue Kleider</t>
-  </si>
-  <si>
-    <t>Vor vielen Jahren lebte ein Kaiser, der so ungeheuer viel auf neue Kleider hielt, daß er all sein Geld dafür ausgab, um recht geputzt zu sein. Er kümmerte sich nicht um seine Soldaten, kümmerte sich nicht um Theater und liebte es nicht, in den Wald zu fahren, außer um seine neuen Kleider zu zeigen. Er hatte einen Rock für jede Stunde des Tages, und ebenso wie man von einem König sagte, er ist im Rat, so sagte man hier immer: "Der Kaiser ist in der Garderobe!"</t>
-  </si>
-  <si>
-    <t>In der großen Stadt, in der er wohnte, ging es sehr munter her. An jedem Tag kamen viele Fremde an, und eines Tages kamen auch zwei Betrüger, die gaben sich für Weber aus und sagten, daß sie das schönste Zeug, was man sich denken könne, zu weben verstanden. Die Farben und das Muster seien nicht allein ungewöhnlich schön, sondern die Kleider, die von dem Zeuge genäht würden, sollten die wunderbare Eigenschaft besitzen, daß sie für jeden Menschen unsichtbar seien, der nicht für sein Amt tauge oder der unverzeihlich dumm sei.</t>
-  </si>
-  <si>
-    <t>,Das wären ja prächtige Kleider', dachte der Kaiser; wenn ich solche hätte, könnte ich ja dahinterkommen, welche Männer in meinem Reiche zu dem Amte, das sie haben, nicht taugen, ich könnte die Klugen von den Dummen unterscheiden! Ja, das Zeug muß sogleich für mich gewebt werden!' Er gab den beiden Betrügern viel Handgeld, damit sie ihre Arbeit beginnen sollten.</t>
-  </si>
-  <si>
-    <t>Alle Menschen in der ganzen Stadt wußten, welche besondere Kraft das Zeug habe, und alle waren begierig zu sehen, wie schlecht oder dumm ihr Nachbar sei.
-,Ich will meinen alten, ehrlichen Minister zu den Webern senden', dachte der Kaiser, er kann am besten beurteilen, wie der Stoff sich ausnimmt, denn er hat Verstand, und keiner versieht sein Amt besser als er!'
-Nun ging der alte, gute Minister in den Saal hinein, wo die zwei Betrüger saßen und an den leeren Webstühlen arbeiteten. ,Gott behüte uns!' dachte der alte Minister und riß die Augen auf. ,Ich kann ja nichts erblicken!' Aber das sagte er nicht.</t>
-  </si>
-  <si>
-    <t>Sie stellten auch zwei Webstühle auf, taten, als ob sie arbeiteten, aber sie hatten nicht das geringste auf dem Stuhle. Trotzdem verlangten sie die feinste Seide und das prächtigste Gold, das steckten sie aber in ihre eigene Tasche und arbeiteten an den leeren Stühlen bis spät in die Nacht hinein.
-,Nun möchte ich doch wissen, wie weit sie mit dem Zeuge sind!' dachte der Kaiser, aber es war ihm beklommen zumute, wenn er daran dachte, daß keiner, der dumm sei oder schlecht zu seinem Amte tauge, es sehen könne. Er glaubte zwar, daß er für sich selbst nichts zu fürchten brauche, aber er wollte doch erst einen andern senden, um zu sehen, wie es damit stehe.</t>
-  </si>
-  <si>
-    <t>Beide Betrüger baten ihn näher zu treten und fragten, ob es nicht ein hübsches Muster und schöne Farben seien. Dann zeigten sie auf den leeren Stuhl, und der arme, alte Minister fuhr fort, die Augen aufzureißen, aber er konnte nichts sehen, denn es war nichts da. ,Herr Gott', dachte er, sollte ich dumm sein? Das habe ich nie geglaubt, und das darf kein Mensch wissen! Sollte ich nicht zu meinem Amte taugen? Nein, es geht nicht an, daß ich erzähle, ich könne das Zeug nicht sehen!'
-"Nun, Sie sagen nichts dazu?" fragte der eine von den Webern.</t>
-  </si>
-  <si>
-    <t>"Oh, es ist niedlich, ganz allerliebst!" antwortete der alte Minister und sah durch seine Brille. "Dieses Muster und diese Farben! – Ja, ich werde dem Kaiser sagen, daß es mir sehr gefällt!"
-"Nun, das freut uns!" sagten beide Weber, und darauf benannten sie die Farben mit Namen und erklärten das seltsame Muster. Der alte Minister merkte gut auf, damit er dasselbe sagen könne, wenn er zum Kaiser zurückkomme, und das tat er auch.
-Nun verlangten die Betrüger mehr Geld, mehr Seide und mehr Gold zum Weben. Sie steckten alles in ihre eigenen Taschen, auf den Webstuhl kam kein Faden, aber sie fuhren fort, wie bisher an den leeren Stühlen zu arbeiten.</t>
-  </si>
-  <si>
-    <t>Sie steckten alles in ihre eigenen Taschen, auf den Webstuhl kam kein Faden, aber sie fuhren fort, wie bisher an den leeren Stühlen zu arbeiten.
-Der Kaiser sandte bald wieder einen anderen tüchtigen Staatsmann hin, um zu sehen, wie es mit dem Weben stehe und ob das Zeug bald fertig sei; es ging ihm aber gerade wie dem ersten, er guckte und guckte; weil aber außer dem Webstuhl nichts da war, so konnte er nichts sehen.
-"Ist das nicht ein ganz besonders prächtiges und hübsches Stück Zeug?" fragten die beiden Betrüger und zeigten und erklärten das prächtige Muster, das gar nicht da war.</t>
-  </si>
-  <si>
-    <t>,Dumm bin ich nicht', dachte der Mann; es ist also mein gutes Amt, zu dem ich nicht tauge! Das wäre seltsam genug, aber das muß man sich nicht merken lassen!' Daher lobte er das Zeug, das er nicht sah, und versicherte ihnen seine Freude über die schönen Farben und das herrliche Muster. "Ja, es ist ganz allerliebst!" sagte er zum Kaiser.
-Alle Menschen in der Stadt sprachen von dem prächtigen Zeuge.</t>
-  </si>
-  <si>
-    <t>Nun wollte der Kaiser es selbst sehen, während es noch auf dem Webstuhl sei. Mit einer ganzen Schar auserwählter Männer, unter denen auch die beiden ehrlichen Staatsmänner waren, die schon früher dagewesen, ging er zu den beiden listigen Betrügern hin, die nun aus allen Kräften webten, aber ohne Faser oder Faden.
-"Ja, ist das nicht prächtig?" sagten die beiden ehrlichen Staatsmänner. "Wollen Eure Majestät sehen, welches Muster, welche Farben?" und dann zeigten sie auf den leeren Webstuhl, denn sie glaubten, daß die andern das Zeug wohl sehen könnten.</t>
-  </si>
-  <si>
-    <t>,Was!' dachte der Kaiser; ich sehe gar nichts! Das ist ja erschrecklich! Bin ich dumm? Tauge ich nicht dazu, Kaiser zu sein? Das wäre das Schrecklichste, was mir begegnen könnte.' "Oh, es ist sehr hübsch", sagte er; "es hat meinen allerhöchsten Beifall!" und er nickte zufrieden und betrachtete den leeren Webstuhl; er wollte nicht sagen, daß er nichts sehen könne. Das ganze Gefolge, was er mit sich hatte, sah und sah, aber es bekam nicht mehr heraus als alle die andern, aber sie sagten gleich wie der Kaiser: "Oh, das ist hübsch!' und sie rieten ihm, diese neuen prächtigen Kleider das erste Mal bei dem großen Feste, das bevorstand, zu tragen.</t>
-  </si>
-  <si>
-    <t>"Es ist herrlich, niedlich, ausgezeichnet!" ging es von Mund zu Mund, und man schien allerseits innig erfreut darüber. Der Kaiser verlieh jedem der Betrüger ein Ritterkreuz, um es in das Knopfloch zu hängen, und den Titel Hofweber.
-Die ganze Nacht vor dem Morgen, an dem das Fest stattfinden sollte, waren die Betrüger auf und hatten sechzehn Lichte angezündet, damit man sie auch recht gut bei ihrer Arbeit beobachten konnte. Die Leute konnten sehen, daß sie stark beschäftigt waren, des Kaisers neue Kleider fertigzumachen. Sie taten, als ob sie das Zeug aus dem Webstuhl nähmen, sie schnitten in die Luft mit großen Scheren, sie nähten mit Nähnadeln ohne Faden und sagten zuletzt: "Sieh, nun sind die Kleider fertig!"</t>
-  </si>
-  <si>
-    <t>Der Kaiser mit seinen vornehmsten Beamten kam selbst, und beide Betrüger hoben den einen Arm in die Höhe, gerade, als ob sie etwas hielten, und sagten: "Seht, hier sind die Beinkleider, hier ist das Kleid, hier ist der Mantel!" und so weiter. "Es ist so leicht wie Spinnwebe; man sollte glauben, man habe nichts auf dem Körper, aber das ist gerade die Schönheit dabei!"
-"Ja!" sagten alle Beamten, aber sie konnten nichts sehen, denn es war nichts da.</t>
-  </si>
-  <si>
-    <t>"Belieben Eure Kaiserliche Majestät Ihre Kleider abzulegen", sagten die Betrüger, "so wollen wir Ihnen die neuen hier vor dem großen Spiegel anziehen!"
-Der Kaiser legte seine Kleider ab, und die Betrüger stellten sich, als ob sie ihm ein jedes Stück der neuen Kleider anzogen, die fertig genäht sein sollten, und der Kaiser wendete und drehte sich vor dem Spiegel.
-"Ei, wie gut sie kleiden, wie herrlich sie sitzen!" sagten alle. "Welches Muster, welche Farben! Das ist ein kostbarer Anzug!" –</t>
-  </si>
-  <si>
-    <t>"Draußen stehen sie mit dem Thronhimmel, der über Eurer Majestät getragen werden soll!" meldete der Oberzeremonienmeister.
-"Seht, ich bin ja fertig!" sagte der Kaiser. "Sitzt es nicht gut?" und dann wendete er sich nochmals zu dem Spiegel; denn es sollte scheinen, als ob er seine Kleider recht betrachte.</t>
-  </si>
-  <si>
-    <t>Die Kammerherren, die das Recht hatten, die Schleppe zu tragen, griffen mit den Händen gegen den Fußboden, als ob sie die Schleppe aufhöben, sie gingen und taten, als hielten sie etwas in der Luft; sie wagten es nicht, es sich merken zu lassen, daß sie nichts sehen konnten.
-So ging der Kaiser unter dem prächtigen Thronhimmel, und alle Menschen auf der Straße und in den Fenstern sprachen: "Wie sind des Kaisers neue Kleider unvergleichlich! Welche Schleppe er am Kleide hat! Wie schön sie sitzt!" Keiner wollte es sich merken lassen, daß er nichts sah; denn dann hätte er ja nicht zu seinem Amte getaugt oder wäre sehr dumm gewesen.</t>
-  </si>
-  <si>
-    <t>Keine Kleider des Kaisers hatten solches Glück gemacht wie diese.
-"Aber er hat ja gar nichts an!" sagte endlich ein kleines Kind. "Hört die Stimme der Unschuld!" sagte der Vater; und der eine zischelte dem andern zu, was das Kind gesagt hatte.
-"Aber er hat ja gar nichts an!" rief zuletzt das ganze Volk. Das ergriff den Kaiser, denn das Volk schien ihm recht zu haben, aber er dachte bei sich: ,Nun muß ich aushalten.' Und die Kammerherren gingen und trugen die Schleppe, die gar nicht da war.</t>
-  </si>
-  <si>
-    <t>Der Alchemist - Kapitel 1</t>
-  </si>
-  <si>
-    <t>Der Jüngling hieß Santiago. Es fing bereits an zu dämmern, als er mit seiner Schafherde zu einer alten, verlassenen Kirche kam. Das Dach war schon vor geraumer Zeit eingestürzt, und ein riesiger Maulbeerbaum wuchs an jener Stelle, wo sich einst die Sakristei befand.
-Er entschloß sich, die Nacht hier zu verbringen. So geleitete er alle Schafe durch die beschädigte Türe und legte einige Bretter quer davor, damit ihm die Tiere während der Nacht nicht entwischen konnten.</t>
-  </si>
-  <si>
-    <t>Zwar gab es keine Wölfe in jener Gegend, aber einmal war ihm eines der Tiere während der Nacht entkommen, und er mußte den ganzen folgenden Tag mit der Suche nach dem verirrten Schäfchen verbringen.
-Danach breitete er seinen Mantel auf dem Fußboden aus, legte sich nieder und nahm das Buch, das er gerade gelesen hatte, als Kopfkissen. Vor dem Einschlafen dachte er daran, daß er in Zukunft dickere Bücher lesen wollte, weil man länger etwas davon hat und weil sie eine bequemere Kopfstütze abgeben.</t>
-  </si>
-  <si>
-    <t>Es war noch finster, als er erwachte. Als er nach oben schaute, sah er die Sterne zwischen den Dachbalken durchscheinen.
-"Eigentlich wollte ich noch weiterschlafen", dachte er bei sich. Wieder hatte er den gleichen Traum gehabt wie vor einer Woche, und wieder war er vor dem Ende aufgewacht.
-Er erhob sich und trank einen Schluck Wein. Dann nahm er seinen Hirtenstab und begann, die Schafe, die noch schliefen, eines nach dem anderen zu wecken. Mehr und mehr wurden die Tiere, wie ihm aufgefallen war, gleichzeitig mit ihm wach, als ob ein geheimnisvoller Gleichklang sein Leben mit dem der Schafe verband, die seit nunmehr zwei Jahren mit ihm übers Land gezogen waren, auf der Suche nach Wasser und Nahrung.</t>
-  </si>
-  <si>
-    <t>"Sie haben sich schon so an mich gewöhnt, daß sie meinen Rhythmus kennen", dachte er. Aber nach kurzer Überlegung kam er zu dem Schluß, daß es auch umgekehrt sein könnte: Er selber hatte sich dem Rhythmus seiner Schafe angepaßt!
-Einige unter den Tieren brauchten etwas länger zum Aufstehen. Der Jüngling weckte sie mit seinem Stab, indem er jedes bei seinem Namen nannte. Immer hatte er den Eindruck, daß die Schafe alles verstanden, was er sagte. Darum las er ihnen auch gelegentlich Abschnitte aus Büchern vor, die ihn besonders beeindruckten, oder er philosophierte über die Einsamkeit und die Freuden eines Schafhirten, oder er kommentierte die letzten Neuigkeiten, die er im den Städten erfahren hatte, durch die er zu ziehen pflegte.</t>
-  </si>
-  <si>
-    <t>Seit zwei Tagen jedoch sprach er beinahe nur noch über eins: die Tochter eines Händlers, die in jener Kleinstadt lebte, welche sie in vier Tagen erreichen würden. Im vorigen Jahr war er das erste Mal bei diesem Handelsmann gewesen, der Besitzer eines Textilgeschäftes war und darauf bestand, daß die Schafe vor seinem Geschäft geschoren würden, um jeden Betrug zu vermeiden. Ein Bekannt er hatte den Laden empfohlen, und so brachte der Hirte seine Schafe jetzt dorthin.</t>
-  </si>
-  <si>
-    <t>BERICHT DER KOMMISSION AN DEN RAT: Fortschrittsbericht über eine Benchmark für die Lernmobilität</t>
-  </si>
-  <si>
-    <t>1. EINFÜHRUNG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In der jüngsten Mitteilung der Kommission „Investieren in Europas Jugend“ werden die positiven Auswirkungen der Lernmobilität auf Beschäftigungsfähigkeit und bürgerschaftliches Engagement hervorgehoben. In einem anderen Land zu lernen, zu studieren oder einer Ausbildung nachzugehen, ist eine einzigartige Erfahrung und kann neue Perspektiven eröffnen. Die Kompetenzen, die im Rahmen einer Mobilitätserfahrung erworben werden, etwa Problemlösungs- und Anpassungsfähigkeit sowie Toleranz und Zuversicht, werden von Arbeitgebern geschätzt und sind in der heutigen Gesellschaft unentbehrlich.
-Die Kommission fördert die Lernmobilität junger Menschen im Rahmen ihrer politischen Konzepte und Programme, die auch eine spezielle Benchmark und die Unterstützung durch das Programm Erasmus+ umfassen. </t>
-  </si>
-  <si>
-    <t>In seinen Schlussfolgerungen zu einer Benchmark für die Lernmobilität (2011/C 372/08) fordert der Rat die Kommission auf, „dem Rat bis Ende 2015 über die Ergebnisse im Hinblick auf eine Überprüfung und gegebenenfalls Überarbeitung der [...] europäischen Benchmark Bericht zu erstatten“.
-Der Rat fordert die Kommission und die Mitgliedstaaten außerdem zur Durchführung einer Reihe weiterer Maßnahmen auf, die sich insbesondere auf Indikatoren für die Mobilität von Studentinnen und Studenten, jungen Menschen und Lehrkräften beziehen. Im Zusammenhang mit diesen Maßnahmen besteht jedoch keine Verpflichtung zur Berichterstattung an den Rat. Hierzu stehen separate Unterlagen der Kommission zur Verfügung, in denen die Maßnahmen eingehender beschrieben werden.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hintergrund der Schlussfolgerungen des Rates von 2011 ist der strategische Rahmen für die europäische Zusammenarbeit auf dem Gebiet der allgemeinen und beruflichen Bildung 2020, in dem die Kommission ersucht wird, „bis Ende 2010 einen Vorschlag für eine Benchmark in diesem Bereich vorzulegen, der sich zunächst auf die physische Mobilität zwischen Ländern im Bereich der Hochschulbildung konzentrieren [...] sollte.“ Den Schlussfolgerungen des Rates ging eine Arbeitsunterlage der Kommissionsdienststellen vom 24. Mai 2011 zur Entwicklung von Benchmarks zu Bildung für Beschäftigungsfähigkeit und zu Mobilität zu Lernzwecken (Dok. 10697/11) voraus.
-Mit dem vorliegenden Bericht wird die Verpflichtung zur Berichterstattung an den Rat über die erzielten Fortschritte bei der Mobilitätsbenchmark im Hinblick auf die Fortsetzung der Arbeit bis 2020 eingelöst. </t>
-  </si>
-  <si>
-    <t>Die aus zwei Indikatoren bestehende Benchmark für die Lernmobilität wird im Anhang der Schlussfolgerungen von 2011 folgendermaßen definiert:
-– „Bis 2020 sollten in der EU durchschnittlich mindestens 20 % der Hochschulabsolventen eine Studien- oder Ausbildungsphase (einschließlich Praktika) im Ausland absolviert haben, die mindestens 15 ECTS-Leistungspunkte abdeckt oder eine Mindestdauer von 3 Monaten umfasst.“
-– „Bis 2020 sollten in der EU durchschnittlich mindestens 6 % der 18- bis 34-Jährigen mit abgeschlossener beruflicher Erstausbildung eine mit der Berufsausbildung zusammenhängende Ausbildungsphase (einschließlich Praktika) von mindestens zwei Wochen oder, sofern im ‚Europass‘ verzeichnet, auch von kürzerer Dauer im Ausland absolviert haben.“</t>
-  </si>
-  <si>
-    <t>Der Schwerpunkt der Benchmark liegt auf der ausgehenden Mobilität, mit anderen Worten auf dem Ausmaß, in dem Menschen ins Ausland gehen, um Lernerfahrungen und Qualifikationen zu erwerben. Innerhalb der EU steht dieses Ziel mit den Grundsätzen der Freizügigkeit von Personen und Arbeitskräften im Binnenmarkt in Verbindung.</t>
-  </si>
-  <si>
-    <t>Die EU-Benchmark misst die Zahl der Absolventen, die während ihres Studiums mobil waren und ihre Qualifikation erfolgreich abgeschlossen haben. Sie hat keinen direkten Bezug zu einem geografischen Gebiet, in den Schlussfolgerungen von 2011 wird jedoch betont: „Lernmobilität bedeutet physische Mobilität einschließlich weltweiter Mobilität.“ Die Messung des Indikators der Benchmark für die Mobilität in der Berufsausbildung wird in der Praxis durch das in den Schlussfolgerungen genannte Instrument (eine Haushaltserhebung bei einer bestimmten, breit angelegten Altersgruppe) begrenzt, während die Quelle für den Indikator im Bereich der Hochschulbildung nicht festgelegt ist.</t>
-  </si>
-  <si>
-    <t>Die Allgemeine Erklärung der Menschenrechte - Präambel</t>
-  </si>
-  <si>
-    <t>Da die Anerkennung der angeborenen Würde und der gleichen und unveräußerlichen Rechte aller Mitglieder der Gemeinschaft der Menschen die Grundlage von Freiheit, Gerechtigkeit und Frieden in der Welt bildet,</t>
-  </si>
-  <si>
-    <t>da die Nichtanerkennung und Verachtung der Menschenrechte zu Akten der Barbarei geführt haben, die das Gewissen der Menschheit mit Empörung erfüllen, und da verkündet worden ist, daß einer Welt, in der die Menschen Rede- und Glaubensfreiheit und Freiheit von Furcht und Not genießen, das höchste Streben des Menschen gilt,</t>
-  </si>
-  <si>
-    <t>da es notwendig ist, die Menschenrechte durch die Herrschaft des Rechtes zu schützen, damit der Mensch nicht gezwungen wird, als letztes Mittel zum Aufstand gegen Tyrannei und Unterdrückung zu greifen,</t>
-  </si>
-  <si>
-    <t>da es notwendig ist, die Entwicklung freundschaftlicher Beziehungen zwischen den Nationen zu fördern,</t>
-  </si>
-  <si>
-    <t>da die Völker der Vereinten Nationen in der Charta ihren Glauben an die grundlegenden Menschenrechte, an die Würde und den Wert der menschlichen Person und an die Gleichberechtigung von Mann und Frau erneut bekräftigt und beschlossen haben, den sozialen Fortschritt und bessere Lebensbedingungen in größerer Freiheit zu fördern,</t>
-  </si>
-  <si>
-    <t>da die Mitgliedstaaten sich verpflichtet haben, in Zusammenarbeit mit den Vereinten Nationen auf die allgemeine Achtung und Einhaltung der Menschenrechte und Grundfreiheiten hinzuwirken,</t>
-  </si>
-  <si>
-    <t>da ein gemeinsames Verständnis dieser Rechte und Freiheiten von größter Wichtigkeit für die volle Erfüllung dieser Verpflichtung ist,</t>
-  </si>
-  <si>
-    <t>verkündet die Generalversammlung diese Allgemeine Erklärung der Menschenrechte als das von allen Völkern und Nationen zu erreichende gemeinsame Ideal, damit jeder einzelne und alle Organe der Gesellschaft sich diese Erklärung stets gegenwärtig halten und sich bemühen, durch Unterricht und Erziehung die Achtung vor diesen Rechten und Freiheiten zu fördern und durch fortschreitende nationale und internationale Maßnahmen ihre allgemeine und tatsächliche Anerkennung und Einhaltung durch die Bevölkerung der Mitgliedstaaten selbst wie auch durch die Bevölkerung der ihrer Hoheitsgewalt unterstehenden Gebiete zu gewährleisten.</t>
-  </si>
-  <si>
-    <t>Willkommen bei MultiplEYE!</t>
-  </si>
-  <si>
-    <t>Der Name „MultiplEYE“ ist ein Wortspiel, das „multilingualism“ (Englisch: Mehrsprachigkeit) oder „multiple languages“ (Englisch: mehrere Sprachen) mit „eye“ (Englisch: Auge) aus „Eye-Tracking“ (Englisch: Blickverfolgung) verbindet. MultiplEYE ist eine von der Europäischen Union finanzierte COST Action. COST Actions sind Forschungsnetzwerke, die von der European Cooperation in Science and Technology, oder kurz COST, unterstützt werden. 
-Als Förderorganisation unterstützt COST unser ständig wachsendes Netzwerk von Forschern in ganz Europa und darüber hinaus, indem es finanzielle Mittel für die Durchführung verschiedener Arten von Networking-Aktivitäten bereitstellt.</t>
-  </si>
-  <si>
-    <t>Zu diesen Aktivitäten gehören Arbeitsgruppentreffen, Weiterbildungskurse, um Expertise an jüngeren Forscher weiterzugeben, und wissenschaftliche Forschungsaufenthalte.
-Der Projekttitel der MultiplEYE COST Action lautet: Ermöglichung der mehrsprachigen Eye-Tracking-Datenerfassung für die menschliche und maschinelle Sprachverarbeitungsforschung (übersetzt aus dem Englischen). Das bedeutet, dass die MultiplEYE COST Action darauf abzielt, ein interdisziplinäres Netzwerk von Forschungsgruppen zu fördern, die an der Erhebung von Augenbewegungsdaten beim Lesen in verschiedenen Sprachen arbeiten.</t>
-  </si>
-  <si>
-    <t>Ziel ist es, die Entwicklung eines großen mehrsprachigen Korpus von Augenbewegungsdaten zu unterstützen und es Forschern zu ermöglichen, Daten zu sammeln, indem sie ihr Expertenwissen aus verschiedenen Disziplinen teilen. Dazu gehören Linguistik, Psychologie, Sprach- und Lesetherapie und Informatik. Diese Datensammlung kann dann verwendet werden, um die menschliche Sprachverarbeitung aus psycholinguistischer Perspektive zu untersuchen, sowie die computergestützte Sprachverarbeitung aus der Perspektive des Maschinellen Lernens zu verbessern und zu evaluieren.</t>
-  </si>
-  <si>
-    <t>Was ist ”Eye-Tracking”?
-Eye-Tracking ist der Prozess, bei dem der Blickpunkt – wohin Sie schauen – und die Augenbewegungen zwischen festen Blickpunkten gemessen werden. Das Gerät, mit dem die Augenpositionen und -bewegungen gemessen werden, wird als Eye-Tracker bezeichnet. Es besteht aus einer Infrarotkamera, die eine Lichtfrequenz verwendet, die das menschliche Auge nicht stört oder verletzt.</t>
-  </si>
-  <si>
-    <t>Mit Hilfe von Bilderkennungsalgorithmen ist der Eye-Tracker in der Lage, Blickpunkte sehr genau zu schätzen, indem er die Position von Kopf und Augen, die Entfernung zum Bildschirm, auf den ein Teilnehmer blickt, und die Position des Eye-Trackers kennt.
-Eye-Tracking ist eine nützliche Technologie für eine Vielzahl von Anwendungen. Beispielsweise kann es dabei helfen, Müdigkeit beim Autofahren zu erkennen oder Anwendungen für Screening- und Trainingszwecke im medizinischen Bereich unterstützen. Eye-Tracking wird auch in der Gaming-Branche, im Marketing und in der Forschung zur Interaktion von Mensch und Maschine eingesetzt.</t>
-  </si>
-  <si>
-    <t>Warum ist Eye-Tracking beim Lesen für unser Projekt besonders interessant?
-Während Sie diese Wörter lesen, folgt der Eye-Tracker Ihren Augenbewegungen über den Text. Dies gibt Aufschluss darüber, wie lange Sie sich einen Text angesehen haben, oder genauer gesagt, wie lange Sie zum Lesen jedes Wortes gebraucht haben, welche Wörter Sie übersprungen haben, bei welchen Wörtern Sie verweilt sind und ob Sie zurückgehen mussten, um die bereits gelesenen Wörter nochmals anzuschauen, um Teile des Textes besser zu verstehen.</t>
-  </si>
-  <si>
-    <t>Während Ihr Gehirn den Inhalt des Textes verarbeitet, spiegeln Ihre Augenbewegungen fast in Echtzeit einen Großteil der dafür benötigten sprachlichen und kognitiven Verarbeitung wider. Die aufgezeichneten Daten sind also eine Goldgrube an Informationen darüber, wie wir die Bedeutung und die grammatikalischen Strukturen eines Textes zusammensetzen. Es zeigt, mit welchen Textstellen wir zu kämpfen haben und welche einfach lesbar sind. Die Forscher können daraus ableiten, welche sprachlichen Faktoren welche Art von Augenbewegungen verursacht haben.</t>
-  </si>
-  <si>
-    <t>Die Motivation hinter MultiplEYE ist, dass Eye-Tracking-Daten noch immer nur spärlich verfügbar sind, insbesondere für kleinere Sprachen. Eine so große Datensammlung ist eine Herausforderung in Bezug auf die Entwicklung und die Vereinbarung des experimentellen Designs, die Komplexität und die Art der Texte, die von den Teilnehmern gelesen werden sollen. Andere Entscheidungen, die weniger relevant erscheinen, aber tatsächlich sehr wichtig sind, betreffen die Schriftart und -größe des Textes, die Reihenfolge der Texte, den Versuchsablauf und die Art und Weise, wie die Daten danach verarbeitet werden.</t>
-  </si>
-  <si>
-    <t>Aber sobald dieser Datensatz fertig ist, wird er es uns ermöglichen, viele Themen im Zusammenhang mit Psycholinguistik und Computerlinguistik zu untersuchen. Beispielsweise können wir das Leseverhalten über verschiedene Sprachen hinweg vergleichen. Hat die Schrift, z.B. das lateinische Alphabet im Vergleich zur kyrillischen oder arabischen Schrift, einen Einfluss auf die Lesezeit? Ein Beispiel für die computergestützte Textverarbeitung könnte die Verwendung von Eye-Tracking-Daten sein, um Anwendungen künstlicher Intelligenz voranzutreiben, die den menschlichen Leseprozess nachahmen. Diese Erkenntnisse könnten verwendet werden, um bessere maschinelle Übersetzungssysteme zu bauen oder um die automatische Extraktion von Schlüsselwörtern aus Texten zu verbessern.</t>
-  </si>
-  <si>
-    <t>Das Erhalten von Eye-Tracking-Daten von vielen verschiedenen Teilnehmern, einschließlich Ihnen selbst, die Texte in vielen verschiedenen Sprachen lesen, wird eine großartige Grundlage für unsere Forschung sein. Sie wird der Hauptfaktor sein, um unser Forschungsnetzwerk zu einem erfolgreichen Unterfangen zu machen.
-Wir hoffen, dass wir den Weg für die Förderung der Forschung in verschiedenen Teilgebieten der Linguistik ebnen können, indem wir eine große Gruppe von Forschern unterstützen und vernetzen.</t>
-  </si>
-  <si>
-    <t>Die Hauptergebnisse der MultiplEYE Action werden ein großer Datensatz mit Blickverfolgungsdaten in vielen Sprachen und eine Plattform für neue Kooperationen sein, die diese Art von Daten nutzen.
-Wenn Sie diesen Text lesen, unterstützen Sie uns bereits, indem Sie uns erlauben, Ihre Augenbewegungen beim Lesen und Verstehen von Sprache zu erfassen und zu analysieren. Vielen Dank!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -863,7 +866,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="66">
     <dxf>
@@ -1613,38 +1616,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9016B68B-E770-4A04-A8EB-C009482E3DEC}">
   <dimension ref="A1:BY28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="81.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="81.33203125" style="1" customWidth="1"/>
-    <col min="8" max="9" width="81.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="73.33203125" style="1" customWidth="1"/>
-    <col min="11" max="15" width="81.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="22" width="81.1640625" style="1" customWidth="1"/>
-    <col min="23" max="25" width="14.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="27" width="14.83203125" style="1" customWidth="1"/>
-    <col min="28" max="28" width="47.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="13.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="31.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="32" width="31.83203125" style="1" customWidth="1"/>
-    <col min="33" max="47" width="16.5" style="1" customWidth="1"/>
-    <col min="48" max="62" width="5.6640625" customWidth="1"/>
-    <col min="63" max="67" width="21.5" customWidth="1"/>
-    <col min="68" max="72" width="19.6640625" style="1" customWidth="1"/>
-    <col min="73" max="75" width="8.6640625" customWidth="1"/>
-    <col min="76" max="76" width="7.5" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="81.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="81.28515625" style="1" customWidth="1"/>
+    <col min="8" max="9" width="81.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="73.28515625" style="1" customWidth="1"/>
+    <col min="11" max="15" width="81.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="22" width="81.140625" style="1" customWidth="1"/>
+    <col min="23" max="25" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="27" width="14.85546875" style="1" customWidth="1"/>
+    <col min="28" max="28" width="47.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="31.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="31.85546875" style="1" customWidth="1"/>
+    <col min="33" max="47" width="16.42578125" style="1" customWidth="1"/>
+    <col min="48" max="62" width="5.7109375" customWidth="1"/>
+    <col min="63" max="67" width="21.42578125" customWidth="1"/>
+    <col min="68" max="72" width="19.7109375" style="1" customWidth="1"/>
+    <col min="73" max="75" width="8.7109375" customWidth="1"/>
+    <col min="76" max="76" width="7.42578125" customWidth="1"/>
     <col min="77" max="77" width="7" customWidth="1"/>
-    <col min="78" max="78" width="24.5" customWidth="1"/>
+    <col min="78" max="78" width="24.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:77" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:77" ht="32.1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1877,345 +1880,348 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:77" ht="128" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:77" ht="128.1">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>102</v>
+        <v>77</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>210</v>
+        <v>78</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>211</v>
+        <v>79</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>212</v>
+        <v>80</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>213</v>
+        <v>81</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>214</v>
+        <v>82</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>215</v>
+        <v>83</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>216</v>
+        <v>84</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>217</v>
+        <v>85</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>218</v>
+        <v>86</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>219</v>
+        <v>87</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>220</v>
+        <v>88</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>221</v>
+        <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:77" ht="112" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:77" ht="111.95">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>201</v>
+        <v>91</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>202</v>
+        <v>92</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>203</v>
+        <v>93</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>204</v>
+        <v>94</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>205</v>
+        <v>95</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>206</v>
+        <v>96</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>207</v>
+        <v>97</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>208</v>
+        <v>98</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>209</v>
+        <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:77" ht="160" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:77" ht="167.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>196</v>
-      </c>
       <c r="G4" s="1" t="s">
-        <v>197</v>
+        <v>105</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>198</v>
+        <v>106</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>199</v>
+        <v>107</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>200</v>
+        <v>108</v>
       </c>
     </row>
-    <row r="5" spans="1:77" ht="144" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:77" ht="144">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>187</v>
+        <v>110</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>188</v>
+        <v>111</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>189</v>
+        <v>112</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>190</v>
+        <v>113</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>191</v>
+        <v>114</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>192</v>
+        <v>115</v>
       </c>
     </row>
-    <row r="6" spans="1:77" ht="128" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:77" ht="128.1">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>169</v>
+        <v>117</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>170</v>
+        <v>118</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>171</v>
+        <v>119</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>172</v>
+        <v>120</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>174</v>
+        <v>121</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>173</v>
+        <v>122</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>175</v>
+        <v>123</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>176</v>
+        <v>124</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>177</v>
+        <v>125</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>178</v>
+        <v>126</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>179</v>
+        <v>127</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>180</v>
+        <v>128</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>181</v>
+        <v>129</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>182</v>
+        <v>130</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>183</v>
+        <v>131</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>184</v>
+        <v>132</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>185</v>
+        <v>133</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>186</v>
+        <v>134</v>
       </c>
     </row>
-    <row r="7" spans="1:77" ht="160" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:77" ht="106.5">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>98</v>
+        <v>135</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>163</v>
+        <v>136</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>164</v>
+        <v>137</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>165</v>
+        <v>138</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>167</v>
+        <v>139</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>140</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>168</v>
+        <v>141</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>142</v>
       </c>
     </row>
-    <row r="8" spans="1:77" ht="144" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:77" ht="152.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>105</v>
+        <v>143</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
     </row>
-    <row r="9" spans="1:77" ht="144" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:77" ht="121.5">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>106</v>
+        <v>150</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
-    <row r="10" spans="1:77" ht="128" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:77" ht="128.1">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>99</v>
+        <v>153</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>135</v>
+        <v>154</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>136</v>
+        <v>155</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>137</v>
+        <v>156</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>138</v>
+        <v>157</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>139</v>
+        <v>158</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>140</v>
+        <v>159</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>141</v>
+        <v>160</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>142</v>
+        <v>161</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>143</v>
+        <v>162</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>144</v>
+        <v>163</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>145</v>
+        <v>164</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>146</v>
+        <v>165</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>147</v>
+        <v>166</v>
       </c>
       <c r="P10" s="3" t="s">
-        <v>148</v>
+        <v>167</v>
       </c>
       <c r="Q10" s="3" t="s">
-        <v>149</v>
+        <v>168</v>
       </c>
       <c r="R10" s="3" t="s">
-        <v>150</v>
+        <v>169</v>
       </c>
       <c r="S10" s="3" t="s">
-        <v>151</v>
+        <v>170</v>
       </c>
       <c r="T10" s="3" t="s">
-        <v>152</v>
+        <v>171</v>
       </c>
       <c r="U10" s="3" t="s">
-        <v>153</v>
+        <v>172</v>
       </c>
       <c r="V10" s="3" t="s">
-        <v>154</v>
+        <v>173</v>
       </c>
     </row>
-    <row r="11" spans="1:77" ht="64" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:77" ht="63.95">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>107</v>
+        <v>174</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="5"/>
@@ -2231,359 +2237,365 @@
       <c r="O11" s="5"/>
       <c r="P11" s="5"/>
       <c r="W11" s="1" t="s">
-        <v>77</v>
+        <v>175</v>
       </c>
       <c r="X11" s="1" t="s">
-        <v>77</v>
+        <v>175</v>
       </c>
       <c r="Y11" s="1" t="s">
-        <v>77</v>
+        <v>175</v>
       </c>
       <c r="AB11" s="1" t="s">
-        <v>78</v>
+        <v>176</v>
       </c>
       <c r="AC11" s="1" t="s">
-        <v>79</v>
+        <v>177</v>
       </c>
       <c r="AD11" s="1" t="s">
-        <v>80</v>
+        <v>178</v>
       </c>
       <c r="AG11" s="1" t="s">
-        <v>81</v>
+        <v>179</v>
       </c>
       <c r="AH11" s="1" t="s">
-        <v>82</v>
+        <v>180</v>
       </c>
       <c r="AI11" s="1" t="s">
-        <v>83</v>
+        <v>181</v>
       </c>
       <c r="AJ11" s="1" t="s">
-        <v>84</v>
+        <v>182</v>
       </c>
       <c r="AK11" s="1" t="s">
-        <v>85</v>
+        <v>183</v>
       </c>
       <c r="AL11" s="1" t="s">
-        <v>86</v>
+        <v>184</v>
       </c>
       <c r="AM11" s="1" t="s">
-        <v>87</v>
+        <v>185</v>
       </c>
       <c r="AN11" s="1" t="s">
-        <v>88</v>
+        <v>186</v>
       </c>
       <c r="AO11" s="1" t="s">
-        <v>89</v>
+        <v>187</v>
       </c>
       <c r="AV11" t="s">
-        <v>90</v>
+        <v>188</v>
       </c>
       <c r="AW11" t="s">
-        <v>91</v>
+        <v>189</v>
       </c>
       <c r="AX11" t="s">
-        <v>92</v>
+        <v>190</v>
       </c>
       <c r="AY11" t="s">
-        <v>79</v>
+        <v>177</v>
       </c>
       <c r="AZ11" t="s">
-        <v>79</v>
+        <v>177</v>
       </c>
       <c r="BA11" t="s">
-        <v>79</v>
+        <v>177</v>
       </c>
       <c r="BB11" t="s">
-        <v>90</v>
+        <v>188</v>
       </c>
       <c r="BC11" t="s">
-        <v>91</v>
+        <v>189</v>
       </c>
       <c r="BD11" t="s">
-        <v>92</v>
+        <v>190</v>
       </c>
       <c r="BK11" t="s">
-        <v>93</v>
+        <v>191</v>
       </c>
       <c r="BL11" t="s">
-        <v>94</v>
+        <v>192</v>
       </c>
       <c r="BM11" t="s">
-        <v>95</v>
+        <v>193</v>
       </c>
       <c r="BP11" s="1" t="s">
-        <v>82</v>
+        <v>180</v>
       </c>
       <c r="BQ11" s="1" t="s">
-        <v>84</v>
+        <v>182</v>
       </c>
       <c r="BR11" s="1" t="s">
-        <v>87</v>
+        <v>185</v>
       </c>
       <c r="BU11" t="s">
-        <v>91</v>
+        <v>189</v>
       </c>
       <c r="BV11" t="s">
-        <v>79</v>
+        <v>177</v>
       </c>
       <c r="BW11" t="s">
-        <v>90</v>
+        <v>188</v>
       </c>
     </row>
-    <row r="12" spans="1:77" ht="160" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:77" ht="137.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>100</v>
+        <v>194</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>122</v>
+        <v>195</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>123</v>
+        <v>196</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>124</v>
+        <v>197</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>126</v>
+        <v>198</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>199</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>127</v>
+        <v>200</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>128</v>
+        <v>201</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>130</v>
+        <v>202</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>203</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>131</v>
+        <v>204</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>132</v>
+        <v>205</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>133</v>
+        <v>206</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>134</v>
+        <v>207</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>209</v>
       </c>
     </row>
-    <row r="13" spans="1:77" ht="128" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:77" ht="152.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>101</v>
+        <v>210</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>108</v>
+        <v>211</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>109</v>
+        <v>212</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>110</v>
+        <v>213</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>111</v>
+        <v>214</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>112</v>
+        <v>215</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>113</v>
+        <v>216</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>114</v>
+        <v>217</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>115</v>
+        <v>218</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>116</v>
+        <v>219</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>117</v>
+        <v>220</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>118</v>
+        <v>221</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>119</v>
+        <v>222</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>120</v>
+        <v>223</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>121</v>
+        <v>224</v>
       </c>
       <c r="W13" s="1" t="s">
-        <v>77</v>
+        <v>175</v>
       </c>
       <c r="X13" s="1" t="s">
-        <v>77</v>
+        <v>175</v>
       </c>
       <c r="Y13" s="1" t="s">
-        <v>77</v>
+        <v>175</v>
       </c>
       <c r="AB13" s="1" t="s">
-        <v>78</v>
+        <v>176</v>
       </c>
       <c r="AC13" s="1" t="s">
-        <v>79</v>
+        <v>177</v>
       </c>
       <c r="AD13" s="1" t="s">
-        <v>80</v>
+        <v>178</v>
       </c>
       <c r="AG13" s="1" t="s">
-        <v>81</v>
+        <v>179</v>
       </c>
       <c r="AH13" s="1" t="s">
-        <v>82</v>
+        <v>180</v>
       </c>
       <c r="AI13" s="1" t="s">
-        <v>83</v>
+        <v>181</v>
       </c>
       <c r="AJ13" s="1" t="s">
-        <v>84</v>
+        <v>182</v>
       </c>
       <c r="AK13" s="1" t="s">
-        <v>85</v>
+        <v>183</v>
       </c>
       <c r="AL13" s="1" t="s">
-        <v>86</v>
+        <v>184</v>
       </c>
       <c r="AM13" s="1" t="s">
-        <v>87</v>
+        <v>185</v>
       </c>
       <c r="AN13" s="1" t="s">
-        <v>88</v>
+        <v>186</v>
       </c>
       <c r="AO13" s="1" t="s">
-        <v>89</v>
+        <v>187</v>
       </c>
       <c r="AV13" t="s">
-        <v>90</v>
+        <v>188</v>
       </c>
       <c r="AW13" t="s">
-        <v>91</v>
+        <v>189</v>
       </c>
       <c r="AX13" t="s">
-        <v>92</v>
+        <v>190</v>
       </c>
       <c r="AY13" t="s">
-        <v>79</v>
+        <v>177</v>
       </c>
       <c r="AZ13" t="s">
-        <v>79</v>
+        <v>177</v>
       </c>
       <c r="BA13" t="s">
-        <v>79</v>
+        <v>177</v>
       </c>
       <c r="BB13" t="s">
-        <v>90</v>
+        <v>188</v>
       </c>
       <c r="BC13" t="s">
-        <v>91</v>
+        <v>189</v>
       </c>
       <c r="BD13" t="s">
-        <v>92</v>
+        <v>190</v>
       </c>
       <c r="BK13" t="s">
-        <v>93</v>
+        <v>191</v>
       </c>
       <c r="BL13" t="s">
-        <v>94</v>
+        <v>192</v>
       </c>
       <c r="BM13" t="s">
-        <v>95</v>
+        <v>193</v>
       </c>
       <c r="BP13" s="1" t="s">
-        <v>82</v>
+        <v>180</v>
       </c>
       <c r="BQ13" s="1" t="s">
-        <v>84</v>
+        <v>182</v>
       </c>
       <c r="BR13" s="1" t="s">
-        <v>87</v>
+        <v>185</v>
       </c>
       <c r="BU13" t="s">
-        <v>91</v>
+        <v>189</v>
       </c>
       <c r="BV13" t="s">
-        <v>79</v>
+        <v>177</v>
       </c>
       <c r="BW13" t="s">
-        <v>90</v>
+        <v>188</v>
       </c>
     </row>
-    <row r="14" spans="1:77" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:77">
       <c r="H14" s="6"/>
     </row>
-    <row r="16" spans="1:77" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:77">
       <c r="M16" s="2"/>
       <c r="R16" s="2"/>
     </row>
-    <row r="18" spans="4:18" x14ac:dyDescent="0.2">
+    <row r="18" spans="4:18">
       <c r="E18" s="2"/>
       <c r="M18" s="2"/>
       <c r="R18" s="2"/>
     </row>
-    <row r="19" spans="4:18" x14ac:dyDescent="0.2">
+    <row r="19" spans="4:18">
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="4:18" x14ac:dyDescent="0.2">
+    <row r="20" spans="4:18">
       <c r="E20" s="2"/>
       <c r="H20" s="2"/>
       <c r="M20" s="2"/>
       <c r="R20" s="2"/>
     </row>
-    <row r="21" spans="4:18" x14ac:dyDescent="0.2">
+    <row r="21" spans="4:18">
       <c r="D21" s="2"/>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="4:18" x14ac:dyDescent="0.2">
+    <row r="22" spans="4:18">
       <c r="E22" s="2"/>
       <c r="H22" s="2"/>
       <c r="M22" s="2"/>
       <c r="R22" s="2"/>
     </row>
-    <row r="23" spans="4:18" x14ac:dyDescent="0.2">
+    <row r="23" spans="4:18">
       <c r="D23" s="2"/>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="4:18" x14ac:dyDescent="0.2">
+    <row r="24" spans="4:18">
       <c r="E24" s="2"/>
       <c r="H24" s="2"/>
       <c r="M24" s="2"/>
     </row>
-    <row r="25" spans="4:18" x14ac:dyDescent="0.2">
+    <row r="25" spans="4:18">
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="4:18" x14ac:dyDescent="0.2">
+    <row r="26" spans="4:18">
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="4:18" x14ac:dyDescent="0.2">
+    <row r="27" spans="4:18">
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="4:18" x14ac:dyDescent="0.2">
+    <row r="28" spans="4:18">
       <c r="H28" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="K13" r:id="rId1" xr:uid="{922F73AC-BAC1-754C-833C-11E8ED4F4A3C}"/>
-    <hyperlink ref="L12" r:id="rId2" xr:uid="{47DA26FC-4703-3540-AB2B-3F0E1DCFDAAB}"/>
-    <hyperlink ref="E12" r:id="rId3" xr:uid="{601CC0F7-B34D-9C45-9B0B-CD155C6EAB69}"/>
+    <hyperlink ref="M12" r:id="rId2" xr:uid="{47DA26FC-4703-3540-AB2B-3F0E1DCFDAAB}"/>
+    <hyperlink ref="F12" r:id="rId3" xr:uid="{601CC0F7-B34D-9C45-9B0B-CD155C6EAB69}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId4"/>
@@ -2599,7 +2611,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2609,9 +2621,5 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D661018-8082-4C74-8BB0-535FAA6BE03A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/DataMashup"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D661018-8082-4C74-8BB0-535FAA6BE03A}"/>
 </file>
</xml_diff>

<commit_message>
added new stimuli files
</commit_message>
<xml_diff>
--- a/stimuli_de/multipleye-stimuli-experiment-de.xlsx
+++ b/stimuli_de/multipleye-stimuli-experiment-de.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tzp466/Documents/research/projects/multipleye/stimulus/final/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{0843B030-2CE3-6047-BC60-3FA1203E2531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0AA467DA-DC13-41F1-82B8-B5EE878024A2}"/>
+  <xr:revisionPtr revIDLastSave="44" documentId="13_ncr:1_{0843B030-2CE3-6047-BC60-3FA1203E2531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B6A1A233-3879-4C89-A7DF-0365B6639CEB}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15760" xr2:uid="{EF339F11-F4DE-4D0A-862E-E00578AF5D2A}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="237">
   <si>
     <t>stimulus_id</t>
   </si>
@@ -375,8 +375,10 @@
 Der Rat fordert die Kommission und die Mitgliedstaaten außerdem zur Durchführung einer Reihe weiterer Maßnahmen auf, die sich insbesondere auf Indikatoren für die Mobilität von Studentinnen und Studenten, jungen Menschen und Lehrkräften beziehen. Im Zusammenhang mit diesen Maßnahmen besteht jedoch keine Verpflichtung zur Berichterstattung an den Rat. Hierzu stehen separate Unterlagen der Kommission zur Verfügung, in denen die Maßnahmen eingehender beschrieben werden.</t>
   </si>
   <si>
-    <t xml:space="preserve">Hintergrund der Schlussfolgerungen des Rates von 2011 ist der strategische Rahmen für die europäische Zusammenarbeit auf dem Gebiet der allgemeinen und beruflichen Bildung 2020, in dem die Kommission ersucht wird, „bis Ende 2010 einen Vorschlag für eine Benchmark in diesem Bereich vorzulegen, der sich zunächst auf die physische Mobilität zwischen Ländern im Bereich der Hochschulbildung konzentrieren [...] sollte.“ Den Schlussfolgerungen des Rates ging eine Arbeitsunterlage der Kommissionsdienststellen vom 24. Mai 2011 zur Entwicklung von Benchmarks zu Bildung für Beschäftigungsfähigkeit und zu Mobilität zu Lernzwecken (Dok. 10697/11) voraus.
-Mit dem vorliegenden Bericht wird die Verpflichtung zur Berichterstattung an den Rat über die erzielten Fortschritte bei der Mobilitätsbenchmark im Hinblick auf die Fortsetzung der Arbeit bis 2020 eingelöst. </t>
+    <t>Hintergrund der Schlussfolgerungen des Rates von 2011 ist der strategische Rahmen für die europäische Zusammenarbeit auf dem Gebiet der allgemeinen und beruflichen Bildung 2020, in dem die Kommission ersucht wird, „bis Ende 2010 einen Vorschlag für eine Benchmark in diesem Bereich vorzulegen, der sich zunächst auf die physische Mobilität zwischen Ländern im Bereich der Hochschulbildung konzentrieren [...] sollte.“ Den Schlussfolgerungen des Rates ging eine Arbeitsunterlage der Kommissionsdienststellen vom 24. Mai 2011 zur Entwicklung von Benchmarks zu Bildung für Beschäftigungsfähigkeit und zu Mobilität zu Lernzwecken (Dok. 10697/11) voraus.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mit dem vorliegenden Bericht wird die Verpflichtung zur Berichterstattung an den Rat über die erzielten Fortschritte bei der Mobilitätsbenchmark im Hinblick auf die Fortsetzung der Arbeit bis 2020 eingelöst. </t>
   </si>
   <si>
     <t>Die aus zwei Indikatoren bestehende Benchmark für die Lernmobilität wird im Anhang der Schlussfolgerungen von 2011 folgendermaßen definiert:
@@ -618,6 +620,44 @@
   </si>
   <si>
     <t>Lit_BrokenApril</t>
+  </si>
+  <si>
+    <t>Der zerrissene April - Kapitel 3</t>
+  </si>
+  <si>
+    <t>Ohne die Hand seiner Frau loszulassen, beugte sich Besian Vorpsi zum Fenster, um nachzusehen, ob die kleine Stadt, in der sie eine halbe Stunde zuvor aufgebrochen waren, die letzte vor der Hochebene im Norden, endlich aus dem Blickfeld entschwunden war. Sanft ansteigende Hänge dehnten sich vor und neben ihnen, ein merkwürdiges Stück Erde, weder Ebene noch Berg noch Plateau.</t>
+  </si>
+  <si>
+    <t>Das Gebirge hatte noch nicht begonnen, doch sein Schatten war schon lange zu spüren. Und obwohl gerade dieser Schatten dem Landstrich den Zugang zur Welt der Berge verwehrte, ließ er doch nicht mehr zu, daß von einer Niederung gesprochen wurde. Niemandsland also, karg und fast unbewohnt.</t>
+  </si>
+  <si>
+    <t>Feine Regentropfen kullerten ab und zu über die Fensterscheiben.
+»Die Verwünschten Almen«, sagte er leise und mit ein wenig bebender Stimme, wie man von etwas spricht, auf dessen Anblick man sich lange gefreut hat. Befriedigt registrierte er, daß die Erwähnung des Namens bei seiner Frau ein feierliches Schaudern auslöste.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Als sie sich herüberbeugte, um hinauszuschauen, roch er den zarten Duft ihres Nackens.
+»Wo?«
+Er wies mit dem Finger auf etwas, doch dort, wo er hinzeigte, waren nur wallende Nebel zu erkennen.
+»Sie sind noch nicht richtig zu sehen«, erklärte er. »Wir sind noch zu weit weg.«
+</t>
+  </si>
+  <si>
+    <t>Sie griff wieder nach seiner Hand und lehnte sich in den Polstern zurück. Die Zeitung, die sie vor der Abfahrt in der kleinen Stadt gekauft hatten (auf der Titelseite war von ihnen die Rede), glitt unter dem Schwanken des Wagens zu Boden, doch sie dachten beide nicht daran, das Blatt wieder aufzuheben. Mit einem verträumten Lächeln dachte sie an die Überschrift: »Eine frohe Überraschung! Der Schriftsteller Besian Vorpsi und seine junge Frau Diana wollen ihre Flitterwochen im nördlichen Hochland verbringen!«</t>
+  </si>
+  <si>
+    <t>Dann ging es etwas verworren weiter. Es war nicht eindeutig zu erschließen, ob der Verfasser des Artikels, ein gewisser A. G. (womöglich ihr gemeinsamer Bekannter Adrian Guma) die Reise nun begrüßte oder sich ein wenig darüber mokierte.</t>
+  </si>
+  <si>
+    <t>Ihr selbst war die Idee zu der Reise ziemlich ausgefallen vorgekommen, als er zwei Wochen vor der Hochzeit zum ersten Mal darüber gesprochen hatte. Du brauchst dich gar nicht zu wundern, hatten ihre Freundinnen gemeint. Wenn man einen so ungewöhnlichen Mann heiratet, bekommt man von ihm eben merkwürdige Dinge zu hören. Aber was heißt das schon. Wir sagen nur: Du Glückliche!</t>
+  </si>
+  <si>
+    <t>Sie war wirklich glücklich. In all den Tagen vor der Hochzeit wurde in Tiranas leidlich mondänen, leidlich kunstsinnigen Kreisen von nichts anderem gesprochen als von ihrer bevorstehenden Reise. Die meisten waren hingerissen: Du kommst aus der realen Welt geradewegs in die Welt der Legenden, mitten in ein wirkliches Epos, wie es sonst fast nirgends in der Welt mehr existiert.</t>
+  </si>
+  <si>
+    <t>Und sie erzählten von Feen und Elfen, von den Rhapsoden, den letzten Homeriden auf der Welt, vom Kanun, der furchtbar war und doch so großartig. Andere wiederum zuckten mit den Schultern ob dieses wunderlichen Einfalls, ihrer Skepsis zaghaft Ausdruck verleihend. Diese betraf vor allem die Frage des Komforts, um so mehr, als es um Flitterwochen, also eine delikate Angelegenheit ging, während es doch in den Alpen noch kalt und die epischen Türme recht steinern waren.</t>
+  </si>
+  <si>
+    <t>Ein kleiner Teil reagierte auf die ganze Sache mit mildem Spott: Geht nur in den Norden, ihr beiden, besucht die Elfen. Vielleicht tut es euch ja gut, vor allem Besian Vorpsi.</t>
   </si>
   <si>
     <t>multiple choice</t>
@@ -844,7 +884,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -854,9 +894,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1616,8 +1653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9016B68B-E770-4A04-A8EB-C009482E3DEC}">
   <dimension ref="A1:BY28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="G3" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1990,31 +2027,34 @@
       <c r="J4" s="1" t="s">
         <v>108</v>
       </c>
+      <c r="K4" s="1" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="5" spans="1:77" ht="144">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:77" ht="128.1">
@@ -2022,61 +2062,61 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:77" ht="106.5">
@@ -2084,28 +2124,28 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:77" ht="152.25">
@@ -2113,25 +2153,25 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:77" ht="121.5">
@@ -2139,13 +2179,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="10" spans="1:77" ht="128.1">
@@ -2153,187 +2193,210 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="P10" s="3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="Q10" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="R10" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="S10" s="3" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="T10" s="3" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="U10" s="3" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="V10" s="3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
-    <row r="11" spans="1:77" ht="63.95">
+    <row r="11" spans="1:77" ht="91.5">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>174</v>
-      </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
-      <c r="O11" s="5"/>
-      <c r="P11" s="5"/>
+        <v>175</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="4"/>
       <c r="W11" s="1" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="X11" s="1" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="Y11" s="1" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="AB11" s="1" t="s">
-        <v>176</v>
+        <v>188</v>
       </c>
       <c r="AC11" s="1" t="s">
-        <v>177</v>
+        <v>189</v>
       </c>
       <c r="AD11" s="1" t="s">
-        <v>178</v>
+        <v>190</v>
       </c>
       <c r="AG11" s="1" t="s">
-        <v>179</v>
+        <v>191</v>
       </c>
       <c r="AH11" s="1" t="s">
-        <v>180</v>
+        <v>192</v>
       </c>
       <c r="AI11" s="1" t="s">
-        <v>181</v>
+        <v>193</v>
       </c>
       <c r="AJ11" s="1" t="s">
-        <v>182</v>
+        <v>194</v>
       </c>
       <c r="AK11" s="1" t="s">
-        <v>183</v>
+        <v>195</v>
       </c>
       <c r="AL11" s="1" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="AM11" s="1" t="s">
-        <v>185</v>
+        <v>197</v>
       </c>
       <c r="AN11" s="1" t="s">
-        <v>186</v>
+        <v>198</v>
       </c>
       <c r="AO11" s="1" t="s">
-        <v>187</v>
+        <v>199</v>
       </c>
       <c r="AV11" t="s">
-        <v>188</v>
+        <v>200</v>
       </c>
       <c r="AW11" t="s">
+        <v>201</v>
+      </c>
+      <c r="AX11" t="s">
+        <v>202</v>
+      </c>
+      <c r="AY11" t="s">
         <v>189</v>
       </c>
-      <c r="AX11" t="s">
-        <v>190</v>
-      </c>
-      <c r="AY11" t="s">
-        <v>177</v>
-      </c>
       <c r="AZ11" t="s">
-        <v>177</v>
+        <v>189</v>
       </c>
       <c r="BA11" t="s">
-        <v>177</v>
+        <v>189</v>
       </c>
       <c r="BB11" t="s">
-        <v>188</v>
+        <v>200</v>
       </c>
       <c r="BC11" t="s">
+        <v>201</v>
+      </c>
+      <c r="BD11" t="s">
+        <v>202</v>
+      </c>
+      <c r="BK11" t="s">
+        <v>203</v>
+      </c>
+      <c r="BL11" t="s">
+        <v>204</v>
+      </c>
+      <c r="BM11" t="s">
+        <v>205</v>
+      </c>
+      <c r="BP11" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="BQ11" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="BR11" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="BU11" t="s">
+        <v>201</v>
+      </c>
+      <c r="BV11" t="s">
         <v>189</v>
       </c>
-      <c r="BD11" t="s">
-        <v>190</v>
-      </c>
-      <c r="BK11" t="s">
-        <v>191</v>
-      </c>
-      <c r="BL11" t="s">
-        <v>192</v>
-      </c>
-      <c r="BM11" t="s">
-        <v>193</v>
-      </c>
-      <c r="BP11" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="BQ11" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="BR11" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="BU11" t="s">
-        <v>189</v>
-      </c>
-      <c r="BV11" t="s">
-        <v>177</v>
-      </c>
       <c r="BW11" t="s">
-        <v>188</v>
+        <v>200</v>
       </c>
     </row>
     <row r="12" spans="1:77" ht="137.25">
@@ -2341,52 +2404,52 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>194</v>
+        <v>206</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>195</v>
+        <v>207</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>196</v>
+        <v>208</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>197</v>
+        <v>209</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>198</v>
+        <v>210</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>199</v>
+        <v>211</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>200</v>
+        <v>212</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>201</v>
+        <v>213</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>202</v>
+        <v>214</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>203</v>
+        <v>215</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>204</v>
+        <v>216</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>205</v>
+        <v>217</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>206</v>
+        <v>218</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>207</v>
+        <v>219</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>208</v>
+        <v>220</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>209</v>
+        <v>221</v>
       </c>
     </row>
     <row r="13" spans="1:77" ht="152.25">
@@ -2394,152 +2457,152 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>210</v>
+        <v>222</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>211</v>
+        <v>223</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>212</v>
+        <v>224</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>213</v>
+        <v>225</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>214</v>
+        <v>226</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>215</v>
+        <v>227</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>216</v>
+        <v>228</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>217</v>
+        <v>229</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>218</v>
+        <v>230</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>219</v>
+        <v>231</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>220</v>
+        <v>232</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>221</v>
+        <v>233</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>222</v>
+        <v>234</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>223</v>
+        <v>235</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>224</v>
+        <v>236</v>
       </c>
       <c r="W13" s="1" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="X13" s="1" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="Y13" s="1" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="AB13" s="1" t="s">
-        <v>176</v>
+        <v>188</v>
       </c>
       <c r="AC13" s="1" t="s">
-        <v>177</v>
+        <v>189</v>
       </c>
       <c r="AD13" s="1" t="s">
-        <v>178</v>
+        <v>190</v>
       </c>
       <c r="AG13" s="1" t="s">
-        <v>179</v>
+        <v>191</v>
       </c>
       <c r="AH13" s="1" t="s">
-        <v>180</v>
+        <v>192</v>
       </c>
       <c r="AI13" s="1" t="s">
-        <v>181</v>
+        <v>193</v>
       </c>
       <c r="AJ13" s="1" t="s">
-        <v>182</v>
+        <v>194</v>
       </c>
       <c r="AK13" s="1" t="s">
-        <v>183</v>
+        <v>195</v>
       </c>
       <c r="AL13" s="1" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="AM13" s="1" t="s">
-        <v>185</v>
+        <v>197</v>
       </c>
       <c r="AN13" s="1" t="s">
-        <v>186</v>
+        <v>198</v>
       </c>
       <c r="AO13" s="1" t="s">
-        <v>187</v>
+        <v>199</v>
       </c>
       <c r="AV13" t="s">
-        <v>188</v>
+        <v>200</v>
       </c>
       <c r="AW13" t="s">
+        <v>201</v>
+      </c>
+      <c r="AX13" t="s">
+        <v>202</v>
+      </c>
+      <c r="AY13" t="s">
         <v>189</v>
       </c>
-      <c r="AX13" t="s">
-        <v>190</v>
-      </c>
-      <c r="AY13" t="s">
-        <v>177</v>
-      </c>
       <c r="AZ13" t="s">
-        <v>177</v>
+        <v>189</v>
       </c>
       <c r="BA13" t="s">
-        <v>177</v>
+        <v>189</v>
       </c>
       <c r="BB13" t="s">
-        <v>188</v>
+        <v>200</v>
       </c>
       <c r="BC13" t="s">
+        <v>201</v>
+      </c>
+      <c r="BD13" t="s">
+        <v>202</v>
+      </c>
+      <c r="BK13" t="s">
+        <v>203</v>
+      </c>
+      <c r="BL13" t="s">
+        <v>204</v>
+      </c>
+      <c r="BM13" t="s">
+        <v>205</v>
+      </c>
+      <c r="BP13" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="BQ13" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="BR13" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="BU13" t="s">
+        <v>201</v>
+      </c>
+      <c r="BV13" t="s">
         <v>189</v>
       </c>
-      <c r="BD13" t="s">
-        <v>190</v>
-      </c>
-      <c r="BK13" t="s">
-        <v>191</v>
-      </c>
-      <c r="BL13" t="s">
-        <v>192</v>
-      </c>
-      <c r="BM13" t="s">
-        <v>193</v>
-      </c>
-      <c r="BP13" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="BQ13" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="BR13" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="BU13" t="s">
-        <v>189</v>
-      </c>
-      <c r="BV13" t="s">
-        <v>177</v>
-      </c>
       <c r="BW13" t="s">
-        <v>188</v>
+        <v>200</v>
       </c>
     </row>
     <row r="14" spans="1:77">
-      <c r="H14" s="6"/>
+      <c r="H14" s="5"/>
     </row>
     <row r="16" spans="1:77">
       <c r="M16" s="2"/>

</xml_diff>